<commit_message>
3ème version du planning
modification avec l'ajout du changement de gravité
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
   <si>
     <t>9h</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>07-08.09.2016 Version 3</t>
+  </si>
+  <si>
+    <t>Ajout du changement de gravité</t>
   </si>
 </sst>
 </file>
@@ -520,7 +523,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -550,15 +553,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
@@ -614,6 +608,20 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -894,11 +902,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BM42"/>
+  <dimension ref="A1:BM43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AZ37" sqref="AZ37"/>
+      <selection pane="topRight" activeCell="AO35" sqref="AO35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,216 +915,216 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="29">
+      <c r="B1" s="84">
         <v>42604</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="29">
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="84">
         <v>42605</v>
       </c>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="29">
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="84">
         <v>42606</v>
       </c>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="29">
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="86"/>
+      <c r="N1" s="84">
         <v>42607</v>
       </c>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="29">
+      <c r="O1" s="85"/>
+      <c r="P1" s="85"/>
+      <c r="Q1" s="86"/>
+      <c r="R1" s="84">
         <v>42608</v>
       </c>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="31"/>
-      <c r="X1" s="29">
+      <c r="S1" s="85"/>
+      <c r="T1" s="85"/>
+      <c r="U1" s="86"/>
+      <c r="X1" s="84">
         <v>42611</v>
       </c>
-      <c r="Y1" s="30"/>
-      <c r="Z1" s="30"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="29">
+      <c r="Y1" s="85"/>
+      <c r="Z1" s="85"/>
+      <c r="AA1" s="86"/>
+      <c r="AB1" s="84">
         <v>42612</v>
       </c>
-      <c r="AC1" s="30"/>
-      <c r="AD1" s="30"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="29">
+      <c r="AC1" s="85"/>
+      <c r="AD1" s="85"/>
+      <c r="AE1" s="86"/>
+      <c r="AF1" s="84">
         <v>42613</v>
       </c>
-      <c r="AG1" s="30"/>
-      <c r="AH1" s="30"/>
-      <c r="AI1" s="31"/>
-      <c r="AJ1" s="29">
+      <c r="AG1" s="85"/>
+      <c r="AH1" s="85"/>
+      <c r="AI1" s="86"/>
+      <c r="AJ1" s="84">
         <v>42614</v>
       </c>
-      <c r="AK1" s="30"/>
-      <c r="AL1" s="30"/>
-      <c r="AM1" s="31"/>
-      <c r="AN1" s="29">
+      <c r="AK1" s="85"/>
+      <c r="AL1" s="85"/>
+      <c r="AM1" s="86"/>
+      <c r="AN1" s="84">
         <v>42615</v>
       </c>
-      <c r="AO1" s="30"/>
-      <c r="AP1" s="30"/>
-      <c r="AQ1" s="31"/>
-      <c r="AT1" s="29">
+      <c r="AO1" s="85"/>
+      <c r="AP1" s="85"/>
+      <c r="AQ1" s="86"/>
+      <c r="AT1" s="84">
         <v>42618</v>
       </c>
-      <c r="AU1" s="30"/>
-      <c r="AV1" s="30"/>
-      <c r="AW1" s="31"/>
-      <c r="AX1" s="29">
+      <c r="AU1" s="85"/>
+      <c r="AV1" s="85"/>
+      <c r="AW1" s="86"/>
+      <c r="AX1" s="84">
         <v>42619</v>
       </c>
-      <c r="AY1" s="30"/>
-      <c r="AZ1" s="30"/>
-      <c r="BA1" s="31"/>
-      <c r="BB1" s="29">
+      <c r="AY1" s="85"/>
+      <c r="AZ1" s="85"/>
+      <c r="BA1" s="86"/>
+      <c r="BB1" s="84">
         <v>42620</v>
       </c>
-      <c r="BC1" s="30"/>
-      <c r="BD1" s="30"/>
-      <c r="BE1" s="31"/>
-      <c r="BF1" s="29">
+      <c r="BC1" s="85"/>
+      <c r="BD1" s="85"/>
+      <c r="BE1" s="86"/>
+      <c r="BF1" s="84">
         <v>42621</v>
       </c>
-      <c r="BG1" s="30"/>
-      <c r="BH1" s="30"/>
-      <c r="BI1" s="31"/>
-      <c r="BJ1" s="29">
+      <c r="BG1" s="85"/>
+      <c r="BH1" s="85"/>
+      <c r="BI1" s="86"/>
+      <c r="BJ1" s="84">
         <v>42622</v>
       </c>
-      <c r="BK1" s="30"/>
-      <c r="BL1" s="30"/>
-      <c r="BM1" s="31"/>
+      <c r="BK1" s="85"/>
+      <c r="BL1" s="85"/>
+      <c r="BM1" s="86"/>
     </row>
     <row r="2" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="33" t="s">
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="33" t="s">
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="33" t="s">
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="32" t="s">
+      <c r="N2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="O2" s="58"/>
-      <c r="P2" s="58"/>
-      <c r="Q2" s="33" t="s">
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="R2" s="32" t="s">
+      <c r="R2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="S2" s="58"/>
-      <c r="T2" s="58"/>
-      <c r="U2" s="33" t="s">
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="X2" s="32" t="s">
+      <c r="X2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="Y2" s="58"/>
-      <c r="Z2" s="58"/>
-      <c r="AA2" s="33" t="s">
+      <c r="Y2" s="55"/>
+      <c r="Z2" s="55"/>
+      <c r="AA2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="AB2" s="32" t="s">
+      <c r="AB2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="AC2" s="58"/>
-      <c r="AD2" s="58"/>
-      <c r="AE2" s="33" t="s">
+      <c r="AC2" s="55"/>
+      <c r="AD2" s="55"/>
+      <c r="AE2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="AF2" s="32" t="s">
+      <c r="AF2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="AG2" s="58"/>
-      <c r="AH2" s="58"/>
-      <c r="AI2" s="33" t="s">
+      <c r="AG2" s="55"/>
+      <c r="AH2" s="55"/>
+      <c r="AI2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="AJ2" s="32" t="s">
+      <c r="AJ2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="AK2" s="58"/>
-      <c r="AL2" s="58"/>
-      <c r="AM2" s="33" t="s">
+      <c r="AK2" s="55"/>
+      <c r="AL2" s="55"/>
+      <c r="AM2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="AN2" s="32" t="s">
+      <c r="AN2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="AO2" s="58"/>
-      <c r="AP2" s="58"/>
-      <c r="AQ2" s="33" t="s">
+      <c r="AO2" s="55"/>
+      <c r="AP2" s="55"/>
+      <c r="AQ2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="AT2" s="32" t="s">
+      <c r="AT2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="AU2" s="58"/>
-      <c r="AV2" s="58"/>
-      <c r="AW2" s="33" t="s">
+      <c r="AU2" s="55"/>
+      <c r="AV2" s="55"/>
+      <c r="AW2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="AX2" s="32" t="s">
+      <c r="AX2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="AY2" s="58"/>
-      <c r="AZ2" s="58"/>
-      <c r="BA2" s="33" t="s">
+      <c r="AY2" s="55"/>
+      <c r="AZ2" s="55"/>
+      <c r="BA2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="BB2" s="32" t="s">
+      <c r="BB2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="BC2" s="58"/>
-      <c r="BD2" s="58"/>
-      <c r="BE2" s="33" t="s">
+      <c r="BC2" s="55"/>
+      <c r="BD2" s="55"/>
+      <c r="BE2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="BF2" s="32" t="s">
+      <c r="BF2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="BG2" s="58"/>
-      <c r="BH2" s="58"/>
-      <c r="BI2" s="33" t="s">
+      <c r="BG2" s="55"/>
+      <c r="BH2" s="55"/>
+      <c r="BI2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="BJ2" s="32" t="s">
+      <c r="BJ2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="BK2" s="58"/>
-      <c r="BL2" s="58"/>
-      <c r="BM2" s="33" t="s">
+      <c r="BK2" s="55"/>
+      <c r="BL2" s="55"/>
+      <c r="BM2" s="30" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1124,1929 +1132,1994 @@
       <c r="A3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="34"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="36"/>
-      <c r="R3" s="56"/>
-      <c r="S3" s="35"/>
-      <c r="T3" s="35"/>
-      <c r="U3" s="36"/>
-      <c r="X3" s="34"/>
-      <c r="Y3" s="35"/>
-      <c r="Z3" s="35"/>
-      <c r="AA3" s="54"/>
-      <c r="AB3" s="34"/>
-      <c r="AC3" s="35"/>
-      <c r="AD3" s="35"/>
-      <c r="AE3" s="36"/>
-      <c r="AF3" s="56"/>
-      <c r="AG3" s="35"/>
-      <c r="AH3" s="35"/>
-      <c r="AI3" s="54"/>
-      <c r="AJ3" s="34"/>
-      <c r="AK3" s="35"/>
-      <c r="AL3" s="35"/>
-      <c r="AM3" s="36"/>
-      <c r="AN3" s="56"/>
-      <c r="AO3" s="35"/>
-      <c r="AP3" s="35"/>
-      <c r="AQ3" s="36"/>
-      <c r="AT3" s="34"/>
-      <c r="AU3" s="35"/>
-      <c r="AV3" s="35"/>
-      <c r="AW3" s="54"/>
-      <c r="AX3" s="34"/>
-      <c r="AY3" s="35"/>
-      <c r="AZ3" s="35"/>
-      <c r="BA3" s="36"/>
-      <c r="BB3" s="56"/>
-      <c r="BC3" s="35"/>
-      <c r="BD3" s="35"/>
-      <c r="BE3" s="54"/>
-      <c r="BF3" s="34"/>
-      <c r="BG3" s="35"/>
-      <c r="BH3" s="35"/>
-      <c r="BI3" s="36"/>
-      <c r="BJ3" s="56"/>
-      <c r="BK3" s="35"/>
-      <c r="BL3" s="35"/>
-      <c r="BM3" s="36"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="33"/>
+      <c r="R3" s="53"/>
+      <c r="S3" s="32"/>
+      <c r="T3" s="32"/>
+      <c r="U3" s="33"/>
+      <c r="X3" s="31"/>
+      <c r="Y3" s="32"/>
+      <c r="Z3" s="32"/>
+      <c r="AA3" s="51"/>
+      <c r="AB3" s="31"/>
+      <c r="AC3" s="32"/>
+      <c r="AD3" s="32"/>
+      <c r="AE3" s="33"/>
+      <c r="AF3" s="53"/>
+      <c r="AG3" s="32"/>
+      <c r="AH3" s="32"/>
+      <c r="AI3" s="51"/>
+      <c r="AJ3" s="31"/>
+      <c r="AK3" s="32"/>
+      <c r="AL3" s="32"/>
+      <c r="AM3" s="33"/>
+      <c r="AN3" s="53"/>
+      <c r="AO3" s="32"/>
+      <c r="AP3" s="32"/>
+      <c r="AQ3" s="33"/>
+      <c r="AT3" s="31"/>
+      <c r="AU3" s="32"/>
+      <c r="AV3" s="32"/>
+      <c r="AW3" s="51"/>
+      <c r="AX3" s="31"/>
+      <c r="AY3" s="32"/>
+      <c r="AZ3" s="32"/>
+      <c r="BA3" s="33"/>
+      <c r="BB3" s="53"/>
+      <c r="BC3" s="32"/>
+      <c r="BD3" s="32"/>
+      <c r="BE3" s="51"/>
+      <c r="BF3" s="31"/>
+      <c r="BG3" s="32"/>
+      <c r="BH3" s="32"/>
+      <c r="BI3" s="33"/>
+      <c r="BJ3" s="53"/>
+      <c r="BK3" s="32"/>
+      <c r="BL3" s="32"/>
+      <c r="BM3" s="33"/>
     </row>
     <row r="4" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="63"/>
-      <c r="C4" s="64"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="61"/>
       <c r="D4" s="1"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="37"/>
+      <c r="F4" s="34"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="38"/>
+      <c r="I4" s="35"/>
       <c r="J4" s="3"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="2"/>
-      <c r="N4" s="37"/>
+      <c r="N4" s="34"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
-      <c r="Q4" s="38"/>
+      <c r="Q4" s="35"/>
       <c r="R4" s="3"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
-      <c r="U4" s="38"/>
-      <c r="X4" s="37"/>
+      <c r="U4" s="35"/>
+      <c r="X4" s="34"/>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
       <c r="AA4" s="2"/>
-      <c r="AB4" s="37"/>
+      <c r="AB4" s="34"/>
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
-      <c r="AE4" s="38"/>
+      <c r="AE4" s="35"/>
       <c r="AF4" s="3"/>
       <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
       <c r="AI4" s="2"/>
-      <c r="AJ4" s="37"/>
+      <c r="AJ4" s="34"/>
       <c r="AK4" s="1"/>
       <c r="AL4" s="1"/>
-      <c r="AM4" s="38"/>
+      <c r="AM4" s="35"/>
       <c r="AN4" s="3"/>
       <c r="AO4" s="1"/>
       <c r="AP4" s="1"/>
-      <c r="AQ4" s="38"/>
-      <c r="AT4" s="37"/>
+      <c r="AQ4" s="35"/>
+      <c r="AT4" s="34"/>
       <c r="AU4" s="1"/>
       <c r="AV4" s="1"/>
       <c r="AW4" s="2"/>
-      <c r="AX4" s="37"/>
+      <c r="AX4" s="34"/>
       <c r="AY4" s="1"/>
       <c r="AZ4" s="1"/>
-      <c r="BA4" s="38"/>
+      <c r="BA4" s="35"/>
       <c r="BB4" s="3"/>
       <c r="BC4" s="1"/>
       <c r="BD4" s="1"/>
       <c r="BE4" s="2"/>
-      <c r="BF4" s="37"/>
+      <c r="BF4" s="34"/>
       <c r="BG4" s="1"/>
       <c r="BH4" s="1"/>
-      <c r="BI4" s="38"/>
+      <c r="BI4" s="35"/>
       <c r="BJ4" s="3"/>
       <c r="BK4" s="1"/>
       <c r="BL4" s="1"/>
-      <c r="BM4" s="38"/>
+      <c r="BM4" s="35"/>
     </row>
     <row r="5" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="37"/>
+      <c r="B5" s="34"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="64"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="61"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="38"/>
+      <c r="I5" s="35"/>
       <c r="J5" s="3"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="2"/>
-      <c r="N5" s="37"/>
+      <c r="N5" s="34"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
-      <c r="Q5" s="38"/>
+      <c r="Q5" s="35"/>
       <c r="R5" s="3"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
-      <c r="U5" s="38"/>
-      <c r="X5" s="37"/>
+      <c r="U5" s="35"/>
+      <c r="X5" s="34"/>
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
       <c r="AA5" s="2"/>
-      <c r="AB5" s="37"/>
+      <c r="AB5" s="34"/>
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
-      <c r="AE5" s="38"/>
+      <c r="AE5" s="35"/>
       <c r="AF5" s="3"/>
       <c r="AG5" s="1"/>
       <c r="AH5" s="1"/>
       <c r="AI5" s="2"/>
-      <c r="AJ5" s="37"/>
+      <c r="AJ5" s="34"/>
       <c r="AK5" s="1"/>
       <c r="AL5" s="1"/>
-      <c r="AM5" s="38"/>
+      <c r="AM5" s="35"/>
       <c r="AN5" s="3"/>
       <c r="AO5" s="1"/>
       <c r="AP5" s="1"/>
-      <c r="AQ5" s="38"/>
-      <c r="AT5" s="37"/>
+      <c r="AQ5" s="35"/>
+      <c r="AT5" s="34"/>
       <c r="AU5" s="1"/>
       <c r="AV5" s="1"/>
       <c r="AW5" s="2"/>
-      <c r="AX5" s="37"/>
+      <c r="AX5" s="34"/>
       <c r="AY5" s="1"/>
       <c r="AZ5" s="1"/>
-      <c r="BA5" s="38"/>
+      <c r="BA5" s="35"/>
       <c r="BB5" s="3"/>
       <c r="BC5" s="1"/>
       <c r="BD5" s="1"/>
       <c r="BE5" s="2"/>
-      <c r="BF5" s="37"/>
+      <c r="BF5" s="34"/>
       <c r="BG5" s="1"/>
       <c r="BH5" s="1"/>
-      <c r="BI5" s="38"/>
+      <c r="BI5" s="35"/>
       <c r="BJ5" s="3"/>
       <c r="BK5" s="1"/>
       <c r="BL5" s="1"/>
-      <c r="BM5" s="38"/>
+      <c r="BM5" s="35"/>
     </row>
     <row r="6" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="37"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="64"/>
-      <c r="I6" s="66"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="61"/>
+      <c r="I6" s="63"/>
       <c r="J6" s="3"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="2"/>
-      <c r="N6" s="37"/>
+      <c r="N6" s="34"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
-      <c r="Q6" s="38"/>
+      <c r="Q6" s="35"/>
       <c r="R6" s="3"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
-      <c r="U6" s="38"/>
-      <c r="X6" s="37"/>
+      <c r="U6" s="35"/>
+      <c r="X6" s="34"/>
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
       <c r="AA6" s="2"/>
-      <c r="AB6" s="37"/>
+      <c r="AB6" s="34"/>
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
-      <c r="AE6" s="38"/>
+      <c r="AE6" s="35"/>
       <c r="AF6" s="3"/>
       <c r="AG6" s="1"/>
       <c r="AH6" s="1"/>
       <c r="AI6" s="2"/>
-      <c r="AJ6" s="37"/>
+      <c r="AJ6" s="34"/>
       <c r="AK6" s="1"/>
       <c r="AL6" s="1"/>
-      <c r="AM6" s="38"/>
+      <c r="AM6" s="35"/>
       <c r="AN6" s="3"/>
       <c r="AO6" s="1"/>
       <c r="AP6" s="1"/>
-      <c r="AQ6" s="38"/>
-      <c r="AT6" s="37"/>
+      <c r="AQ6" s="35"/>
+      <c r="AT6" s="34"/>
       <c r="AU6" s="1"/>
       <c r="AV6" s="1"/>
       <c r="AW6" s="2"/>
-      <c r="AX6" s="37"/>
+      <c r="AX6" s="34"/>
       <c r="AY6" s="1"/>
       <c r="AZ6" s="1"/>
-      <c r="BA6" s="38"/>
+      <c r="BA6" s="35"/>
       <c r="BB6" s="3"/>
       <c r="BC6" s="1"/>
       <c r="BD6" s="1"/>
       <c r="BE6" s="2"/>
-      <c r="BF6" s="37"/>
+      <c r="BF6" s="34"/>
       <c r="BG6" s="1"/>
       <c r="BH6" s="1"/>
-      <c r="BI6" s="38"/>
+      <c r="BI6" s="35"/>
       <c r="BJ6" s="3"/>
       <c r="BK6" s="1"/>
       <c r="BL6" s="1"/>
-      <c r="BM6" s="38"/>
+      <c r="BM6" s="35"/>
     </row>
     <row r="7" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="37"/>
+      <c r="B7" s="34"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="37"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="67"/>
-      <c r="K7" s="64"/>
-      <c r="L7" s="64"/>
-      <c r="M7" s="65"/>
-      <c r="N7" s="63"/>
-      <c r="O7" s="64"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="64"/>
+      <c r="K7" s="61"/>
+      <c r="L7" s="61"/>
+      <c r="M7" s="62"/>
+      <c r="N7" s="60"/>
+      <c r="O7" s="61"/>
       <c r="P7" s="1"/>
-      <c r="Q7" s="38"/>
+      <c r="Q7" s="35"/>
       <c r="R7" s="3"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
-      <c r="U7" s="38"/>
-      <c r="X7" s="37"/>
+      <c r="U7" s="35"/>
+      <c r="X7" s="34"/>
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
       <c r="AA7" s="2"/>
-      <c r="AB7" s="37"/>
+      <c r="AB7" s="34"/>
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
-      <c r="AE7" s="38"/>
+      <c r="AE7" s="35"/>
       <c r="AF7" s="3"/>
       <c r="AG7" s="1"/>
       <c r="AH7" s="1"/>
       <c r="AI7" s="2"/>
-      <c r="AJ7" s="37"/>
+      <c r="AJ7" s="34"/>
       <c r="AK7" s="1"/>
       <c r="AL7" s="1"/>
-      <c r="AM7" s="38"/>
+      <c r="AM7" s="35"/>
       <c r="AN7" s="3"/>
       <c r="AO7" s="1"/>
       <c r="AP7" s="1"/>
-      <c r="AQ7" s="38"/>
-      <c r="AT7" s="37"/>
+      <c r="AQ7" s="35"/>
+      <c r="AT7" s="34"/>
       <c r="AU7" s="1"/>
       <c r="AV7" s="1"/>
       <c r="AW7" s="2"/>
-      <c r="AX7" s="37"/>
+      <c r="AX7" s="34"/>
       <c r="AY7" s="1"/>
       <c r="AZ7" s="1"/>
-      <c r="BA7" s="38"/>
+      <c r="BA7" s="35"/>
       <c r="BB7" s="3"/>
       <c r="BC7" s="1"/>
       <c r="BD7" s="1"/>
       <c r="BE7" s="2"/>
-      <c r="BF7" s="37"/>
+      <c r="BF7" s="34"/>
       <c r="BG7" s="1"/>
       <c r="BH7" s="1"/>
-      <c r="BI7" s="38"/>
+      <c r="BI7" s="35"/>
       <c r="BJ7" s="3"/>
       <c r="BK7" s="1"/>
       <c r="BL7" s="1"/>
-      <c r="BM7" s="38"/>
+      <c r="BM7" s="35"/>
     </row>
     <row r="8" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="37"/>
+      <c r="B8" s="34"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="37"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="38"/>
+      <c r="I8" s="35"/>
       <c r="J8" s="3"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="2"/>
-      <c r="N8" s="37"/>
+      <c r="N8" s="34"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
-      <c r="Q8" s="38"/>
+      <c r="Q8" s="35"/>
       <c r="R8" s="3"/>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
-      <c r="U8" s="38"/>
-      <c r="X8" s="37"/>
+      <c r="U8" s="35"/>
+      <c r="X8" s="34"/>
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
       <c r="AA8" s="2"/>
-      <c r="AB8" s="37"/>
+      <c r="AB8" s="34"/>
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
-      <c r="AE8" s="38"/>
+      <c r="AE8" s="35"/>
       <c r="AF8" s="3"/>
       <c r="AG8" s="1"/>
       <c r="AH8" s="1"/>
       <c r="AI8" s="2"/>
-      <c r="AJ8" s="37"/>
+      <c r="AJ8" s="34"/>
       <c r="AK8" s="1"/>
       <c r="AL8" s="1"/>
-      <c r="AM8" s="38"/>
-      <c r="AN8" s="67"/>
-      <c r="AO8" s="64"/>
-      <c r="AP8" s="64"/>
-      <c r="AQ8" s="66"/>
-      <c r="AT8" s="63"/>
-      <c r="AU8" s="64"/>
-      <c r="AV8" s="64"/>
-      <c r="AW8" s="65"/>
-      <c r="AX8" s="63"/>
-      <c r="AY8" s="64"/>
-      <c r="AZ8" s="64"/>
-      <c r="BA8" s="66"/>
+      <c r="AM8" s="35"/>
+      <c r="AN8" s="64"/>
+      <c r="AO8" s="61"/>
+      <c r="AP8" s="61"/>
+      <c r="AQ8" s="63"/>
+      <c r="AT8" s="60"/>
+      <c r="AU8" s="61"/>
+      <c r="AV8" s="61"/>
+      <c r="AW8" s="62"/>
+      <c r="AX8" s="60"/>
+      <c r="AY8" s="61"/>
+      <c r="AZ8" s="61"/>
+      <c r="BA8" s="63"/>
       <c r="BB8" s="3"/>
       <c r="BC8" s="1"/>
       <c r="BD8" s="1"/>
       <c r="BE8" s="2"/>
-      <c r="BF8" s="37"/>
+      <c r="BF8" s="34"/>
       <c r="BG8" s="1"/>
       <c r="BH8" s="1"/>
-      <c r="BI8" s="38"/>
+      <c r="BI8" s="35"/>
       <c r="BJ8" s="3"/>
       <c r="BK8" s="1"/>
       <c r="BL8" s="1"/>
-      <c r="BM8" s="38"/>
+      <c r="BM8" s="35"/>
     </row>
     <row r="9" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="37"/>
+      <c r="B9" s="34"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="37"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="38"/>
+      <c r="I9" s="35"/>
       <c r="J9" s="3"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="2"/>
-      <c r="N9" s="37"/>
+      <c r="N9" s="34"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
-      <c r="Q9" s="38"/>
+      <c r="Q9" s="35"/>
       <c r="R9" s="3"/>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
-      <c r="U9" s="38"/>
-      <c r="X9" s="37"/>
+      <c r="U9" s="35"/>
+      <c r="X9" s="34"/>
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
       <c r="AA9" s="2"/>
-      <c r="AB9" s="37"/>
+      <c r="AB9" s="34"/>
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
-      <c r="AE9" s="38"/>
+      <c r="AE9" s="35"/>
       <c r="AF9" s="3"/>
       <c r="AG9" s="1"/>
       <c r="AH9" s="1"/>
       <c r="AI9" s="2"/>
-      <c r="AJ9" s="37"/>
+      <c r="AJ9" s="34"/>
       <c r="AK9" s="1"/>
       <c r="AL9" s="1"/>
-      <c r="AM9" s="38"/>
+      <c r="AM9" s="35"/>
       <c r="AN9" s="3"/>
       <c r="AO9" s="1"/>
       <c r="AP9" s="1"/>
-      <c r="AQ9" s="38"/>
-      <c r="AT9" s="37"/>
+      <c r="AQ9" s="35"/>
+      <c r="AT9" s="34"/>
       <c r="AU9" s="1"/>
       <c r="AV9" s="1"/>
       <c r="AW9" s="2"/>
-      <c r="AX9" s="37"/>
+      <c r="AX9" s="34"/>
       <c r="AY9" s="1"/>
       <c r="AZ9" s="1"/>
-      <c r="BA9" s="38"/>
-      <c r="BB9" s="67"/>
-      <c r="BC9" s="64"/>
-      <c r="BD9" s="64"/>
-      <c r="BE9" s="65"/>
-      <c r="BF9" s="63"/>
-      <c r="BG9" s="64"/>
-      <c r="BH9" s="64"/>
-      <c r="BI9" s="66"/>
-      <c r="BJ9" s="67"/>
-      <c r="BK9" s="64"/>
-      <c r="BL9" s="64"/>
-      <c r="BM9" s="66"/>
+      <c r="BA9" s="35"/>
+      <c r="BB9" s="64"/>
+      <c r="BC9" s="61"/>
+      <c r="BD9" s="61"/>
+      <c r="BE9" s="62"/>
+      <c r="BF9" s="60"/>
+      <c r="BG9" s="61"/>
+      <c r="BH9" s="61"/>
+      <c r="BI9" s="63"/>
+      <c r="BJ9" s="64"/>
+      <c r="BK9" s="61"/>
+      <c r="BL9" s="61"/>
+      <c r="BM9" s="63"/>
     </row>
     <row r="10" spans="1:65" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="39"/>
+      <c r="B10" s="36"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="8"/>
-      <c r="F10" s="39"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
-      <c r="I10" s="40"/>
+      <c r="I10" s="37"/>
       <c r="J10" s="9"/>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
       <c r="M10" s="8"/>
-      <c r="N10" s="39"/>
+      <c r="N10" s="36"/>
       <c r="O10" s="7"/>
       <c r="P10" s="7"/>
-      <c r="Q10" s="40"/>
+      <c r="Q10" s="37"/>
       <c r="R10" s="9"/>
       <c r="S10" s="7"/>
       <c r="T10" s="7"/>
-      <c r="U10" s="40"/>
-      <c r="X10" s="39"/>
+      <c r="U10" s="37"/>
+      <c r="X10" s="36"/>
       <c r="Y10" s="7"/>
       <c r="Z10" s="7"/>
       <c r="AA10" s="8"/>
-      <c r="AB10" s="39"/>
+      <c r="AB10" s="36"/>
       <c r="AC10" s="7"/>
       <c r="AD10" s="7"/>
-      <c r="AE10" s="40"/>
+      <c r="AE10" s="37"/>
       <c r="AF10" s="9"/>
       <c r="AG10" s="7"/>
       <c r="AH10" s="7"/>
       <c r="AI10" s="8"/>
-      <c r="AJ10" s="39"/>
+      <c r="AJ10" s="36"/>
       <c r="AK10" s="7"/>
       <c r="AL10" s="7"/>
-      <c r="AM10" s="40"/>
+      <c r="AM10" s="37"/>
       <c r="AN10" s="9"/>
       <c r="AO10" s="7"/>
       <c r="AP10" s="7"/>
-      <c r="AQ10" s="40"/>
-      <c r="AT10" s="39"/>
+      <c r="AQ10" s="37"/>
+      <c r="AT10" s="36"/>
       <c r="AU10" s="7"/>
       <c r="AV10" s="7"/>
       <c r="AW10" s="8"/>
-      <c r="AX10" s="39"/>
+      <c r="AX10" s="36"/>
       <c r="AY10" s="7"/>
       <c r="AZ10" s="7"/>
-      <c r="BA10" s="40"/>
+      <c r="BA10" s="37"/>
       <c r="BB10" s="9"/>
       <c r="BC10" s="7"/>
       <c r="BD10" s="7"/>
       <c r="BE10" s="8"/>
-      <c r="BF10" s="39"/>
+      <c r="BF10" s="36"/>
       <c r="BG10" s="7"/>
       <c r="BH10" s="7"/>
-      <c r="BI10" s="40"/>
+      <c r="BI10" s="37"/>
       <c r="BJ10" s="9"/>
       <c r="BK10" s="7"/>
       <c r="BL10" s="7"/>
-      <c r="BM10" s="40"/>
+      <c r="BM10" s="37"/>
     </row>
     <row r="11" spans="1:65" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="41"/>
+      <c r="B11" s="38"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
       <c r="E11" s="11"/>
-      <c r="F11" s="41"/>
+      <c r="F11" s="38"/>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
-      <c r="I11" s="42"/>
+      <c r="I11" s="39"/>
       <c r="J11" s="12"/>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
       <c r="M11" s="11"/>
-      <c r="N11" s="41"/>
+      <c r="N11" s="38"/>
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
-      <c r="Q11" s="42"/>
+      <c r="Q11" s="39"/>
       <c r="R11" s="12"/>
       <c r="S11" s="10"/>
       <c r="T11" s="10"/>
-      <c r="U11" s="42"/>
-      <c r="X11" s="41"/>
+      <c r="U11" s="39"/>
+      <c r="X11" s="38"/>
       <c r="Y11" s="10"/>
       <c r="Z11" s="10"/>
       <c r="AA11" s="11"/>
-      <c r="AB11" s="41"/>
+      <c r="AB11" s="38"/>
       <c r="AC11" s="10"/>
       <c r="AD11" s="10"/>
-      <c r="AE11" s="42"/>
+      <c r="AE11" s="39"/>
       <c r="AF11" s="12"/>
       <c r="AG11" s="10"/>
       <c r="AH11" s="10"/>
       <c r="AI11" s="11"/>
-      <c r="AJ11" s="41"/>
+      <c r="AJ11" s="38"/>
       <c r="AK11" s="10"/>
       <c r="AL11" s="10"/>
-      <c r="AM11" s="42"/>
+      <c r="AM11" s="39"/>
       <c r="AN11" s="12"/>
       <c r="AO11" s="10"/>
       <c r="AP11" s="10"/>
-      <c r="AQ11" s="42"/>
-      <c r="AT11" s="41"/>
+      <c r="AQ11" s="39"/>
+      <c r="AT11" s="38"/>
       <c r="AU11" s="10"/>
       <c r="AV11" s="10"/>
       <c r="AW11" s="11"/>
-      <c r="AX11" s="41"/>
+      <c r="AX11" s="38"/>
       <c r="AY11" s="10"/>
       <c r="AZ11" s="10"/>
-      <c r="BA11" s="42"/>
+      <c r="BA11" s="39"/>
       <c r="BB11" s="12"/>
       <c r="BC11" s="10"/>
       <c r="BD11" s="10"/>
       <c r="BE11" s="11"/>
-      <c r="BF11" s="41"/>
+      <c r="BF11" s="38"/>
       <c r="BG11" s="10"/>
       <c r="BH11" s="10"/>
-      <c r="BI11" s="42"/>
+      <c r="BI11" s="39"/>
       <c r="BJ11" s="12"/>
       <c r="BK11" s="10"/>
       <c r="BL11" s="10"/>
-      <c r="BM11" s="42"/>
+      <c r="BM11" s="39"/>
     </row>
     <row r="12" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="37"/>
+      <c r="B12" s="34"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="37"/>
+      <c r="F12" s="34"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="38"/>
+      <c r="I12" s="35"/>
       <c r="J12" s="3"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="2"/>
-      <c r="N12" s="37"/>
+      <c r="N12" s="34"/>
       <c r="O12" s="1"/>
-      <c r="P12" s="69"/>
-      <c r="Q12" s="70"/>
+      <c r="P12" s="66"/>
+      <c r="Q12" s="67"/>
       <c r="R12" s="3"/>
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
-      <c r="U12" s="38"/>
-      <c r="X12" s="37"/>
+      <c r="U12" s="35"/>
+      <c r="X12" s="34"/>
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
       <c r="AA12" s="2"/>
-      <c r="AB12" s="37"/>
+      <c r="AB12" s="34"/>
       <c r="AC12" s="1"/>
       <c r="AD12" s="1"/>
-      <c r="AE12" s="38"/>
+      <c r="AE12" s="35"/>
       <c r="AF12" s="3"/>
       <c r="AG12" s="1"/>
       <c r="AH12" s="1"/>
       <c r="AI12" s="2"/>
-      <c r="AJ12" s="37"/>
+      <c r="AJ12" s="34"/>
       <c r="AK12" s="1"/>
       <c r="AL12" s="1"/>
-      <c r="AM12" s="38"/>
+      <c r="AM12" s="35"/>
       <c r="AN12" s="3"/>
       <c r="AO12" s="1"/>
       <c r="AP12" s="1"/>
-      <c r="AQ12" s="38"/>
-      <c r="AT12" s="37"/>
+      <c r="AQ12" s="35"/>
+      <c r="AT12" s="34"/>
       <c r="AU12" s="1"/>
       <c r="AV12" s="1"/>
       <c r="AW12" s="2"/>
-      <c r="AX12" s="37"/>
+      <c r="AX12" s="34"/>
       <c r="AY12" s="1"/>
       <c r="AZ12" s="1"/>
-      <c r="BA12" s="38"/>
+      <c r="BA12" s="35"/>
       <c r="BB12" s="3"/>
       <c r="BC12" s="1"/>
       <c r="BD12" s="1"/>
       <c r="BE12" s="2"/>
-      <c r="BF12" s="37"/>
+      <c r="BF12" s="34"/>
       <c r="BG12" s="1"/>
       <c r="BH12" s="1"/>
-      <c r="BI12" s="38"/>
+      <c r="BI12" s="35"/>
       <c r="BJ12" s="3"/>
       <c r="BK12" s="1"/>
       <c r="BL12" s="1"/>
-      <c r="BM12" s="38"/>
+      <c r="BM12" s="35"/>
     </row>
     <row r="13" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="37"/>
+      <c r="B13" s="34"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="37"/>
+      <c r="F13" s="34"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="38"/>
+      <c r="I13" s="35"/>
       <c r="J13" s="3"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="2"/>
-      <c r="N13" s="37"/>
+      <c r="N13" s="34"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
-      <c r="Q13" s="38"/>
-      <c r="R13" s="71"/>
-      <c r="S13" s="69"/>
-      <c r="T13" s="69"/>
-      <c r="U13" s="70"/>
-      <c r="X13" s="68"/>
-      <c r="Y13" s="69"/>
-      <c r="Z13" s="69"/>
-      <c r="AA13" s="75"/>
-      <c r="AB13" s="68"/>
-      <c r="AC13" s="69"/>
-      <c r="AD13" s="69"/>
-      <c r="AE13" s="70"/>
+      <c r="Q13" s="35"/>
+      <c r="R13" s="68"/>
+      <c r="S13" s="66"/>
+      <c r="T13" s="66"/>
+      <c r="U13" s="67"/>
+      <c r="X13" s="65"/>
+      <c r="Y13" s="66"/>
+      <c r="Z13" s="66"/>
+      <c r="AA13" s="72"/>
+      <c r="AB13" s="65"/>
+      <c r="AC13" s="66"/>
+      <c r="AD13" s="66"/>
+      <c r="AE13" s="67"/>
       <c r="AF13" s="3"/>
       <c r="AG13" s="1"/>
       <c r="AH13" s="1"/>
       <c r="AI13" s="2"/>
-      <c r="AJ13" s="37"/>
+      <c r="AJ13" s="34"/>
       <c r="AK13" s="1"/>
       <c r="AL13" s="1"/>
-      <c r="AM13" s="38"/>
+      <c r="AM13" s="35"/>
       <c r="AN13" s="3"/>
       <c r="AO13" s="1"/>
       <c r="AP13" s="1"/>
-      <c r="AQ13" s="38"/>
-      <c r="AT13" s="37"/>
+      <c r="AQ13" s="35"/>
+      <c r="AT13" s="34"/>
       <c r="AU13" s="1"/>
       <c r="AV13" s="1"/>
       <c r="AW13" s="2"/>
-      <c r="AX13" s="37"/>
+      <c r="AX13" s="34"/>
       <c r="AY13" s="1"/>
       <c r="AZ13" s="1"/>
-      <c r="BA13" s="38"/>
+      <c r="BA13" s="35"/>
       <c r="BB13" s="3"/>
       <c r="BC13" s="1"/>
       <c r="BD13" s="1"/>
       <c r="BE13" s="2"/>
-      <c r="BF13" s="37"/>
+      <c r="BF13" s="34"/>
       <c r="BG13" s="1"/>
       <c r="BH13" s="1"/>
-      <c r="BI13" s="38"/>
+      <c r="BI13" s="35"/>
       <c r="BJ13" s="3"/>
       <c r="BK13" s="1"/>
       <c r="BL13" s="1"/>
-      <c r="BM13" s="38"/>
+      <c r="BM13" s="35"/>
     </row>
     <row r="14" spans="1:65" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="43"/>
+      <c r="B14" s="40"/>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
       <c r="E14" s="23"/>
-      <c r="F14" s="43"/>
+      <c r="F14" s="40"/>
       <c r="G14" s="22"/>
       <c r="H14" s="22"/>
-      <c r="I14" s="44"/>
+      <c r="I14" s="41"/>
       <c r="J14" s="24"/>
       <c r="K14" s="22"/>
       <c r="L14" s="22"/>
       <c r="M14" s="23"/>
-      <c r="N14" s="43"/>
+      <c r="N14" s="40"/>
       <c r="O14" s="22"/>
       <c r="P14" s="22"/>
-      <c r="Q14" s="44"/>
+      <c r="Q14" s="41"/>
       <c r="R14" s="24"/>
       <c r="S14" s="22"/>
       <c r="T14" s="22"/>
-      <c r="U14" s="44"/>
-      <c r="X14" s="43"/>
+      <c r="U14" s="41"/>
+      <c r="X14" s="40"/>
       <c r="Y14" s="22"/>
       <c r="Z14" s="22"/>
       <c r="AA14" s="23"/>
-      <c r="AB14" s="43"/>
+      <c r="AB14" s="40"/>
       <c r="AC14" s="22"/>
       <c r="AD14" s="22"/>
-      <c r="AE14" s="44"/>
+      <c r="AE14" s="41"/>
       <c r="AF14" s="24"/>
       <c r="AG14" s="22"/>
       <c r="AH14" s="22"/>
       <c r="AI14" s="23"/>
-      <c r="AJ14" s="43"/>
+      <c r="AJ14" s="40"/>
       <c r="AK14" s="22"/>
       <c r="AL14" s="22"/>
-      <c r="AM14" s="44"/>
+      <c r="AM14" s="41"/>
       <c r="AN14" s="24"/>
       <c r="AO14" s="22"/>
       <c r="AP14" s="22"/>
-      <c r="AQ14" s="44"/>
-      <c r="AT14" s="43"/>
+      <c r="AQ14" s="41"/>
+      <c r="AT14" s="40"/>
       <c r="AU14" s="22"/>
       <c r="AV14" s="22"/>
       <c r="AW14" s="23"/>
-      <c r="AX14" s="43"/>
+      <c r="AX14" s="40"/>
       <c r="AY14" s="22"/>
       <c r="AZ14" s="22"/>
-      <c r="BA14" s="44"/>
+      <c r="BA14" s="41"/>
       <c r="BB14" s="24"/>
       <c r="BC14" s="22"/>
       <c r="BD14" s="22"/>
       <c r="BE14" s="23"/>
-      <c r="BF14" s="43"/>
+      <c r="BF14" s="40"/>
       <c r="BG14" s="22"/>
       <c r="BH14" s="22"/>
-      <c r="BI14" s="44"/>
+      <c r="BI14" s="41"/>
       <c r="BJ14" s="24"/>
       <c r="BK14" s="22"/>
       <c r="BL14" s="22"/>
-      <c r="BM14" s="44"/>
+      <c r="BM14" s="41"/>
     </row>
     <row r="15" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="37"/>
+      <c r="B15" s="34"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="37"/>
+      <c r="F15" s="34"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="38"/>
+      <c r="I15" s="35"/>
       <c r="J15" s="3"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="2"/>
-      <c r="N15" s="37"/>
+      <c r="N15" s="34"/>
       <c r="O15" s="1"/>
-      <c r="P15" s="73"/>
-      <c r="Q15" s="74"/>
-      <c r="R15" s="76"/>
-      <c r="S15" s="73"/>
-      <c r="T15" s="73"/>
-      <c r="U15" s="74"/>
-      <c r="X15" s="72"/>
-      <c r="Y15" s="73"/>
-      <c r="Z15" s="73"/>
-      <c r="AA15" s="80"/>
-      <c r="AB15" s="37"/>
+      <c r="P15" s="70"/>
+      <c r="Q15" s="71"/>
+      <c r="R15" s="73"/>
+      <c r="S15" s="70"/>
+      <c r="T15" s="70"/>
+      <c r="U15" s="71"/>
+      <c r="X15" s="69"/>
+      <c r="Y15" s="70"/>
+      <c r="Z15" s="70"/>
+      <c r="AA15" s="77"/>
+      <c r="AB15" s="34"/>
       <c r="AC15" s="1"/>
       <c r="AD15" s="1"/>
-      <c r="AE15" s="38"/>
+      <c r="AE15" s="35"/>
       <c r="AF15" s="3"/>
       <c r="AG15" s="1"/>
       <c r="AH15" s="1"/>
       <c r="AI15" s="2"/>
-      <c r="AJ15" s="37"/>
+      <c r="AJ15" s="34"/>
       <c r="AK15" s="1"/>
       <c r="AL15" s="1"/>
-      <c r="AM15" s="38"/>
+      <c r="AM15" s="35"/>
       <c r="AN15" s="3"/>
       <c r="AO15" s="1"/>
       <c r="AP15" s="1"/>
-      <c r="AQ15" s="38"/>
-      <c r="AT15" s="37"/>
+      <c r="AQ15" s="35"/>
+      <c r="AT15" s="34"/>
       <c r="AU15" s="1"/>
       <c r="AV15" s="1"/>
       <c r="AW15" s="2"/>
-      <c r="AX15" s="37"/>
+      <c r="AX15" s="34"/>
       <c r="AY15" s="1"/>
       <c r="AZ15" s="1"/>
-      <c r="BA15" s="38"/>
+      <c r="BA15" s="35"/>
       <c r="BB15" s="3"/>
       <c r="BC15" s="1"/>
       <c r="BD15" s="1"/>
       <c r="BE15" s="2"/>
-      <c r="BF15" s="37"/>
+      <c r="BF15" s="34"/>
       <c r="BG15" s="1"/>
       <c r="BH15" s="1"/>
-      <c r="BI15" s="38"/>
+      <c r="BI15" s="35"/>
       <c r="BJ15" s="3"/>
       <c r="BK15" s="1"/>
       <c r="BL15" s="1"/>
-      <c r="BM15" s="38"/>
+      <c r="BM15" s="35"/>
     </row>
     <row r="16" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="37"/>
+      <c r="B16" s="34"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="37"/>
+      <c r="F16" s="34"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="38"/>
+      <c r="I16" s="35"/>
       <c r="J16" s="3"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="2"/>
-      <c r="N16" s="37"/>
+      <c r="N16" s="34"/>
       <c r="O16" s="1"/>
-      <c r="P16" s="77"/>
-      <c r="Q16" s="78"/>
-      <c r="R16" s="79"/>
-      <c r="S16" s="77"/>
-      <c r="T16" s="77"/>
-      <c r="U16" s="78"/>
-      <c r="X16" s="37"/>
+      <c r="P16" s="74"/>
+      <c r="Q16" s="75"/>
+      <c r="R16" s="76"/>
+      <c r="S16" s="74"/>
+      <c r="T16" s="74"/>
+      <c r="U16" s="75"/>
+      <c r="X16" s="34"/>
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
       <c r="AA16" s="2"/>
-      <c r="AB16" s="37"/>
+      <c r="AB16" s="34"/>
       <c r="AC16" s="1"/>
       <c r="AD16" s="1"/>
-      <c r="AE16" s="38"/>
+      <c r="AE16" s="35"/>
       <c r="AF16" s="3"/>
       <c r="AG16" s="1"/>
       <c r="AH16" s="1"/>
       <c r="AI16" s="2"/>
-      <c r="AJ16" s="37"/>
+      <c r="AJ16" s="34"/>
       <c r="AK16" s="1"/>
       <c r="AL16" s="1"/>
-      <c r="AM16" s="38"/>
+      <c r="AM16" s="35"/>
       <c r="AN16" s="3"/>
       <c r="AO16" s="1"/>
       <c r="AP16" s="1"/>
-      <c r="AQ16" s="38"/>
-      <c r="AT16" s="37"/>
+      <c r="AQ16" s="35"/>
+      <c r="AT16" s="34"/>
       <c r="AU16" s="1"/>
       <c r="AV16" s="1"/>
       <c r="AW16" s="2"/>
-      <c r="AX16" s="37"/>
+      <c r="AX16" s="34"/>
       <c r="AY16" s="1"/>
       <c r="AZ16" s="1"/>
-      <c r="BA16" s="38"/>
+      <c r="BA16" s="35"/>
       <c r="BB16" s="3"/>
       <c r="BC16" s="1"/>
       <c r="BD16" s="1"/>
       <c r="BE16" s="2"/>
-      <c r="BF16" s="37"/>
+      <c r="BF16" s="34"/>
       <c r="BG16" s="1"/>
       <c r="BH16" s="1"/>
-      <c r="BI16" s="38"/>
+      <c r="BI16" s="35"/>
       <c r="BJ16" s="3"/>
       <c r="BK16" s="1"/>
       <c r="BL16" s="1"/>
-      <c r="BM16" s="38"/>
+      <c r="BM16" s="35"/>
     </row>
     <row r="17" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="37"/>
+      <c r="B17" s="34"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="37"/>
+      <c r="F17" s="34"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="38"/>
+      <c r="I17" s="35"/>
       <c r="J17" s="3"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="2"/>
-      <c r="N17" s="37"/>
+      <c r="N17" s="34"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
-      <c r="Q17" s="38"/>
+      <c r="Q17" s="35"/>
       <c r="R17" s="3"/>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
-      <c r="U17" s="38"/>
-      <c r="X17" s="81"/>
-      <c r="Y17" s="77"/>
-      <c r="Z17" s="77"/>
-      <c r="AA17" s="82"/>
-      <c r="AB17" s="81"/>
-      <c r="AC17" s="77"/>
+      <c r="U17" s="35"/>
+      <c r="X17" s="78"/>
+      <c r="Y17" s="74"/>
+      <c r="Z17" s="74"/>
+      <c r="AA17" s="79"/>
+      <c r="AB17" s="78"/>
+      <c r="AC17" s="74"/>
       <c r="AD17" s="1"/>
-      <c r="AE17" s="38"/>
+      <c r="AE17" s="35"/>
       <c r="AF17" s="3"/>
       <c r="AG17" s="1"/>
       <c r="AH17" s="1"/>
       <c r="AI17" s="2"/>
-      <c r="AJ17" s="37"/>
+      <c r="AJ17" s="34"/>
       <c r="AK17" s="1"/>
       <c r="AL17" s="1"/>
-      <c r="AM17" s="38"/>
+      <c r="AM17" s="35"/>
       <c r="AN17" s="3"/>
       <c r="AO17" s="1"/>
       <c r="AP17" s="1"/>
-      <c r="AQ17" s="38"/>
-      <c r="AT17" s="37"/>
+      <c r="AQ17" s="35"/>
+      <c r="AT17" s="34"/>
       <c r="AU17" s="1"/>
       <c r="AV17" s="1"/>
       <c r="AW17" s="2"/>
-      <c r="AX17" s="37"/>
+      <c r="AX17" s="34"/>
       <c r="AY17" s="1"/>
       <c r="AZ17" s="1"/>
-      <c r="BA17" s="38"/>
+      <c r="BA17" s="35"/>
       <c r="BB17" s="3"/>
       <c r="BC17" s="1"/>
       <c r="BD17" s="1"/>
       <c r="BE17" s="2"/>
-      <c r="BF17" s="37"/>
+      <c r="BF17" s="34"/>
       <c r="BG17" s="1"/>
       <c r="BH17" s="1"/>
-      <c r="BI17" s="38"/>
+      <c r="BI17" s="35"/>
       <c r="BJ17" s="3"/>
       <c r="BK17" s="1"/>
       <c r="BL17" s="1"/>
-      <c r="BM17" s="38"/>
+      <c r="BM17" s="35"/>
     </row>
     <row r="18" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="37"/>
+      <c r="B18" s="34"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
-      <c r="F18" s="37"/>
+      <c r="F18" s="34"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="38"/>
+      <c r="I18" s="35"/>
       <c r="J18" s="3"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="2"/>
-      <c r="N18" s="37"/>
+      <c r="N18" s="34"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
-      <c r="Q18" s="38"/>
+      <c r="Q18" s="35"/>
       <c r="R18" s="3"/>
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
-      <c r="U18" s="38"/>
-      <c r="X18" s="37"/>
+      <c r="U18" s="35"/>
+      <c r="X18" s="34"/>
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
       <c r="AA18" s="2"/>
-      <c r="AB18" s="37"/>
+      <c r="AB18" s="34"/>
       <c r="AC18" s="1"/>
-      <c r="AD18" s="77"/>
-      <c r="AE18" s="78"/>
-      <c r="AF18" s="79"/>
-      <c r="AG18" s="77"/>
-      <c r="AH18" s="77"/>
-      <c r="AI18" s="82"/>
-      <c r="AJ18" s="37"/>
+      <c r="AD18" s="74"/>
+      <c r="AE18" s="75"/>
+      <c r="AF18" s="76"/>
+      <c r="AG18" s="74"/>
+      <c r="AH18" s="74"/>
+      <c r="AI18" s="79"/>
+      <c r="AJ18" s="34"/>
       <c r="AK18" s="1"/>
       <c r="AL18" s="1"/>
-      <c r="AM18" s="38"/>
+      <c r="AM18" s="35"/>
       <c r="AN18" s="3"/>
       <c r="AO18" s="1"/>
       <c r="AP18" s="1"/>
-      <c r="AQ18" s="38"/>
-      <c r="AT18" s="37"/>
+      <c r="AQ18" s="35"/>
+      <c r="AT18" s="34"/>
       <c r="AU18" s="1"/>
       <c r="AV18" s="1"/>
       <c r="AW18" s="2"/>
-      <c r="AX18" s="37"/>
+      <c r="AX18" s="34"/>
       <c r="AY18" s="1"/>
       <c r="AZ18" s="1"/>
-      <c r="BA18" s="38"/>
+      <c r="BA18" s="35"/>
       <c r="BB18" s="3"/>
       <c r="BC18" s="1"/>
       <c r="BD18" s="1"/>
       <c r="BE18" s="2"/>
-      <c r="BF18" s="37"/>
+      <c r="BF18" s="34"/>
       <c r="BG18" s="1"/>
       <c r="BH18" s="1"/>
-      <c r="BI18" s="38"/>
+      <c r="BI18" s="35"/>
       <c r="BJ18" s="3"/>
       <c r="BK18" s="1"/>
       <c r="BL18" s="1"/>
-      <c r="BM18" s="38"/>
+      <c r="BM18" s="35"/>
     </row>
     <row r="19" spans="1:65" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="45"/>
+      <c r="B19" s="42"/>
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
       <c r="E19" s="15"/>
-      <c r="F19" s="45"/>
+      <c r="F19" s="42"/>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
-      <c r="I19" s="46"/>
+      <c r="I19" s="43"/>
       <c r="J19" s="16"/>
       <c r="K19" s="14"/>
       <c r="L19" s="14"/>
       <c r="M19" s="15"/>
-      <c r="N19" s="45"/>
+      <c r="N19" s="42"/>
       <c r="O19" s="14"/>
       <c r="P19" s="14"/>
-      <c r="Q19" s="46"/>
+      <c r="Q19" s="43"/>
       <c r="R19" s="16"/>
       <c r="S19" s="14"/>
       <c r="T19" s="14"/>
-      <c r="U19" s="46"/>
-      <c r="X19" s="45"/>
+      <c r="U19" s="43"/>
+      <c r="X19" s="42"/>
       <c r="Y19" s="14"/>
       <c r="Z19" s="14"/>
       <c r="AA19" s="15"/>
-      <c r="AB19" s="45"/>
+      <c r="AB19" s="42"/>
       <c r="AC19" s="14"/>
       <c r="AD19" s="14"/>
-      <c r="AE19" s="46"/>
+      <c r="AE19" s="43"/>
       <c r="AF19" s="16"/>
       <c r="AG19" s="14"/>
       <c r="AH19" s="14"/>
       <c r="AI19" s="15"/>
-      <c r="AJ19" s="45"/>
+      <c r="AJ19" s="42"/>
       <c r="AK19" s="14"/>
       <c r="AL19" s="14"/>
-      <c r="AM19" s="46"/>
+      <c r="AM19" s="43"/>
       <c r="AN19" s="16"/>
       <c r="AO19" s="14"/>
       <c r="AP19" s="14"/>
-      <c r="AQ19" s="46"/>
-      <c r="AT19" s="45"/>
+      <c r="AQ19" s="43"/>
+      <c r="AT19" s="42"/>
       <c r="AU19" s="14"/>
       <c r="AV19" s="14"/>
       <c r="AW19" s="15"/>
-      <c r="AX19" s="45"/>
+      <c r="AX19" s="42"/>
       <c r="AY19" s="14"/>
       <c r="AZ19" s="14"/>
-      <c r="BA19" s="46"/>
+      <c r="BA19" s="43"/>
       <c r="BB19" s="16"/>
       <c r="BC19" s="14"/>
       <c r="BD19" s="14"/>
       <c r="BE19" s="15"/>
-      <c r="BF19" s="45"/>
+      <c r="BF19" s="42"/>
       <c r="BG19" s="14"/>
       <c r="BH19" s="14"/>
-      <c r="BI19" s="46"/>
+      <c r="BI19" s="43"/>
       <c r="BJ19" s="16"/>
       <c r="BK19" s="14"/>
       <c r="BL19" s="14"/>
-      <c r="BM19" s="46"/>
+      <c r="BM19" s="43"/>
     </row>
     <row r="20" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="37"/>
+      <c r="B20" s="34"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="37"/>
+      <c r="F20" s="34"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="38"/>
+      <c r="I20" s="35"/>
       <c r="J20" s="3"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="2"/>
-      <c r="N20" s="37"/>
+      <c r="N20" s="34"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
-      <c r="Q20" s="38"/>
+      <c r="Q20" s="35"/>
       <c r="R20" s="3"/>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
-      <c r="U20" s="38"/>
-      <c r="X20" s="37"/>
+      <c r="U20" s="35"/>
+      <c r="X20" s="34"/>
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
       <c r="AA20" s="2"/>
-      <c r="AB20" s="72"/>
-      <c r="AC20" s="73"/>
-      <c r="AD20" s="73"/>
-      <c r="AE20" s="74"/>
-      <c r="AF20" s="76"/>
-      <c r="AG20" s="73"/>
-      <c r="AH20" s="73"/>
-      <c r="AI20" s="80"/>
-      <c r="AJ20" s="37"/>
+      <c r="AB20" s="69"/>
+      <c r="AC20" s="70"/>
+      <c r="AD20" s="70"/>
+      <c r="AE20" s="71"/>
+      <c r="AF20" s="73"/>
+      <c r="AG20" s="70"/>
+      <c r="AH20" s="70"/>
+      <c r="AI20" s="77"/>
+      <c r="AJ20" s="34"/>
       <c r="AK20" s="1"/>
       <c r="AL20" s="1"/>
-      <c r="AM20" s="38"/>
+      <c r="AM20" s="35"/>
       <c r="AN20" s="3"/>
       <c r="AO20" s="1"/>
       <c r="AP20" s="1"/>
-      <c r="AQ20" s="38"/>
-      <c r="AT20" s="37"/>
+      <c r="AQ20" s="35"/>
+      <c r="AT20" s="34"/>
       <c r="AU20" s="1"/>
       <c r="AV20" s="1"/>
       <c r="AW20" s="2"/>
-      <c r="AX20" s="37"/>
+      <c r="AX20" s="34"/>
       <c r="AY20" s="1"/>
       <c r="AZ20" s="1"/>
-      <c r="BA20" s="38"/>
+      <c r="BA20" s="35"/>
       <c r="BB20" s="3"/>
       <c r="BC20" s="1"/>
       <c r="BD20" s="1"/>
       <c r="BE20" s="2"/>
-      <c r="BF20" s="37"/>
+      <c r="BF20" s="34"/>
       <c r="BG20" s="1"/>
       <c r="BH20" s="1"/>
-      <c r="BI20" s="38"/>
+      <c r="BI20" s="35"/>
       <c r="BJ20" s="3"/>
       <c r="BK20" s="1"/>
       <c r="BL20" s="1"/>
-      <c r="BM20" s="38"/>
+      <c r="BM20" s="35"/>
     </row>
     <row r="21" spans="1:65" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="47"/>
+      <c r="B21" s="44"/>
       <c r="C21" s="18"/>
       <c r="D21" s="18"/>
       <c r="E21" s="19"/>
-      <c r="F21" s="47"/>
+      <c r="F21" s="44"/>
       <c r="G21" s="18"/>
       <c r="H21" s="18"/>
-      <c r="I21" s="48"/>
+      <c r="I21" s="45"/>
       <c r="J21" s="20"/>
       <c r="K21" s="18"/>
       <c r="L21" s="18"/>
       <c r="M21" s="19"/>
-      <c r="N21" s="47"/>
+      <c r="N21" s="44"/>
       <c r="O21" s="18"/>
       <c r="P21" s="18"/>
-      <c r="Q21" s="48"/>
+      <c r="Q21" s="45"/>
       <c r="R21" s="20"/>
       <c r="S21" s="18"/>
       <c r="T21" s="18"/>
-      <c r="U21" s="48"/>
-      <c r="X21" s="47"/>
+      <c r="U21" s="45"/>
+      <c r="X21" s="44"/>
       <c r="Y21" s="18"/>
       <c r="Z21" s="18"/>
       <c r="AA21" s="19"/>
-      <c r="AB21" s="47"/>
+      <c r="AB21" s="44"/>
       <c r="AC21" s="18"/>
       <c r="AD21" s="18"/>
-      <c r="AE21" s="48"/>
+      <c r="AE21" s="45"/>
       <c r="AF21" s="20"/>
       <c r="AG21" s="18"/>
       <c r="AH21" s="18"/>
       <c r="AI21" s="19"/>
-      <c r="AJ21" s="47"/>
+      <c r="AJ21" s="44"/>
       <c r="AK21" s="18"/>
       <c r="AL21" s="18"/>
-      <c r="AM21" s="48"/>
+      <c r="AM21" s="45"/>
       <c r="AN21" s="20"/>
       <c r="AO21" s="18"/>
       <c r="AP21" s="18"/>
-      <c r="AQ21" s="48"/>
-      <c r="AT21" s="47"/>
+      <c r="AQ21" s="45"/>
+      <c r="AT21" s="44"/>
       <c r="AU21" s="18"/>
       <c r="AV21" s="18"/>
       <c r="AW21" s="19"/>
-      <c r="AX21" s="47"/>
+      <c r="AX21" s="44"/>
       <c r="AY21" s="18"/>
       <c r="AZ21" s="18"/>
-      <c r="BA21" s="48"/>
+      <c r="BA21" s="45"/>
       <c r="BB21" s="20"/>
       <c r="BC21" s="18"/>
       <c r="BD21" s="18"/>
       <c r="BE21" s="19"/>
-      <c r="BF21" s="47"/>
+      <c r="BF21" s="44"/>
       <c r="BG21" s="18"/>
       <c r="BH21" s="18"/>
-      <c r="BI21" s="48"/>
+      <c r="BI21" s="45"/>
       <c r="BJ21" s="20"/>
       <c r="BK21" s="18"/>
       <c r="BL21" s="18"/>
-      <c r="BM21" s="48"/>
+      <c r="BM21" s="45"/>
     </row>
     <row r="22" spans="1:65" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="43"/>
+      <c r="B22" s="40"/>
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
       <c r="E22" s="23"/>
-      <c r="F22" s="43"/>
+      <c r="F22" s="40"/>
       <c r="G22" s="22"/>
       <c r="H22" s="22"/>
-      <c r="I22" s="44"/>
+      <c r="I22" s="41"/>
       <c r="J22" s="24"/>
       <c r="K22" s="22"/>
       <c r="L22" s="22"/>
       <c r="M22" s="23"/>
-      <c r="N22" s="43"/>
+      <c r="N22" s="40"/>
       <c r="O22" s="22"/>
       <c r="P22" s="22"/>
-      <c r="Q22" s="44"/>
+      <c r="Q22" s="41"/>
       <c r="R22" s="24"/>
       <c r="S22" s="22"/>
       <c r="T22" s="22"/>
-      <c r="U22" s="44"/>
-      <c r="X22" s="43"/>
+      <c r="U22" s="41"/>
+      <c r="X22" s="40"/>
       <c r="Y22" s="22"/>
       <c r="Z22" s="22"/>
       <c r="AA22" s="23"/>
-      <c r="AB22" s="43"/>
+      <c r="AB22" s="40"/>
       <c r="AC22" s="22"/>
       <c r="AD22" s="22"/>
-      <c r="AE22" s="44"/>
+      <c r="AE22" s="41"/>
       <c r="AF22" s="24"/>
       <c r="AG22" s="22"/>
       <c r="AH22" s="22"/>
       <c r="AI22" s="23"/>
-      <c r="AJ22" s="43"/>
+      <c r="AJ22" s="40"/>
       <c r="AK22" s="22"/>
       <c r="AL22" s="22"/>
-      <c r="AM22" s="44"/>
+      <c r="AM22" s="41"/>
       <c r="AN22" s="24"/>
       <c r="AO22" s="22"/>
       <c r="AP22" s="22"/>
-      <c r="AQ22" s="44"/>
-      <c r="AT22" s="43"/>
+      <c r="AQ22" s="41"/>
+      <c r="AT22" s="40"/>
       <c r="AU22" s="22"/>
       <c r="AV22" s="22"/>
       <c r="AW22" s="23"/>
-      <c r="AX22" s="43"/>
+      <c r="AX22" s="40"/>
       <c r="AY22" s="22"/>
       <c r="AZ22" s="22"/>
-      <c r="BA22" s="44"/>
+      <c r="BA22" s="41"/>
       <c r="BB22" s="24"/>
       <c r="BC22" s="22"/>
       <c r="BD22" s="22"/>
       <c r="BE22" s="23"/>
-      <c r="BF22" s="43"/>
+      <c r="BF22" s="40"/>
       <c r="BG22" s="22"/>
       <c r="BH22" s="22"/>
-      <c r="BI22" s="44"/>
+      <c r="BI22" s="41"/>
       <c r="BJ22" s="24"/>
       <c r="BK22" s="22"/>
       <c r="BL22" s="22"/>
-      <c r="BM22" s="44"/>
+      <c r="BM22" s="41"/>
     </row>
     <row r="23" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="37"/>
+      <c r="B23" s="34"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="37"/>
+      <c r="F23" s="34"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
-      <c r="I23" s="38"/>
+      <c r="I23" s="35"/>
       <c r="J23" s="3"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="2"/>
-      <c r="N23" s="37"/>
+      <c r="N23" s="34"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
-      <c r="Q23" s="38"/>
+      <c r="Q23" s="35"/>
       <c r="R23" s="3"/>
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
-      <c r="U23" s="38"/>
-      <c r="X23" s="37"/>
+      <c r="U23" s="35"/>
+      <c r="X23" s="34"/>
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
       <c r="AA23" s="2"/>
-      <c r="AB23" s="37"/>
+      <c r="AB23" s="34"/>
       <c r="AC23" s="1"/>
       <c r="AD23" s="1"/>
-      <c r="AE23" s="38"/>
+      <c r="AE23" s="35"/>
       <c r="AF23" s="3"/>
       <c r="AG23" s="1"/>
       <c r="AH23" s="1"/>
       <c r="AI23" s="2"/>
-      <c r="AJ23" s="81"/>
-      <c r="AK23" s="77"/>
-      <c r="AL23" s="77"/>
-      <c r="AM23" s="78"/>
-      <c r="AN23" s="79"/>
-      <c r="AO23" s="77"/>
+      <c r="AJ23" s="78"/>
+      <c r="AK23" s="74"/>
+      <c r="AL23" s="74"/>
+      <c r="AM23" s="75"/>
+      <c r="AN23" s="76"/>
+      <c r="AO23" s="74"/>
       <c r="AP23" s="1"/>
-      <c r="AQ23" s="38"/>
-      <c r="AT23" s="37"/>
+      <c r="AQ23" s="35"/>
+      <c r="AT23" s="34"/>
       <c r="AU23" s="1"/>
       <c r="AV23" s="1"/>
       <c r="AW23" s="2"/>
-      <c r="AX23" s="37"/>
+      <c r="AX23" s="34"/>
       <c r="AY23" s="1"/>
       <c r="AZ23" s="1"/>
-      <c r="BA23" s="38"/>
+      <c r="BA23" s="35"/>
       <c r="BB23" s="3"/>
       <c r="BC23" s="1"/>
       <c r="BD23" s="1"/>
       <c r="BE23" s="2"/>
-      <c r="BF23" s="37"/>
+      <c r="BF23" s="34"/>
       <c r="BG23" s="1"/>
       <c r="BH23" s="1"/>
-      <c r="BI23" s="38"/>
+      <c r="BI23" s="35"/>
       <c r="BJ23" s="3"/>
       <c r="BK23" s="1"/>
       <c r="BL23" s="1"/>
-      <c r="BM23" s="38"/>
+      <c r="BM23" s="35"/>
     </row>
     <row r="24" spans="1:65" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="45"/>
+      <c r="B24" s="42"/>
       <c r="C24" s="14"/>
       <c r="D24" s="14"/>
       <c r="E24" s="15"/>
-      <c r="F24" s="45"/>
+      <c r="F24" s="42"/>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
-      <c r="I24" s="46"/>
+      <c r="I24" s="43"/>
       <c r="J24" s="16"/>
       <c r="K24" s="14"/>
       <c r="L24" s="14"/>
       <c r="M24" s="15"/>
-      <c r="N24" s="45"/>
+      <c r="N24" s="42"/>
       <c r="O24" s="14"/>
       <c r="P24" s="14"/>
-      <c r="Q24" s="46"/>
+      <c r="Q24" s="43"/>
       <c r="R24" s="16"/>
       <c r="S24" s="14"/>
       <c r="T24" s="14"/>
-      <c r="U24" s="46"/>
-      <c r="X24" s="45"/>
+      <c r="U24" s="43"/>
+      <c r="X24" s="42"/>
       <c r="Y24" s="14"/>
       <c r="Z24" s="14"/>
       <c r="AA24" s="15"/>
-      <c r="AB24" s="45"/>
+      <c r="AB24" s="42"/>
       <c r="AC24" s="14"/>
       <c r="AD24" s="14"/>
-      <c r="AE24" s="46"/>
+      <c r="AE24" s="43"/>
       <c r="AF24" s="16"/>
       <c r="AG24" s="14"/>
       <c r="AH24" s="14"/>
       <c r="AI24" s="15"/>
-      <c r="AJ24" s="45"/>
+      <c r="AJ24" s="42"/>
       <c r="AK24" s="14"/>
       <c r="AL24" s="14"/>
-      <c r="AM24" s="46"/>
+      <c r="AM24" s="43"/>
       <c r="AN24" s="16"/>
       <c r="AO24" s="14"/>
       <c r="AP24" s="14"/>
-      <c r="AQ24" s="46"/>
-      <c r="AT24" s="45"/>
+      <c r="AQ24" s="43"/>
+      <c r="AT24" s="42"/>
       <c r="AU24" s="14"/>
       <c r="AV24" s="14"/>
       <c r="AW24" s="15"/>
-      <c r="AX24" s="45"/>
+      <c r="AX24" s="42"/>
       <c r="AY24" s="14"/>
       <c r="AZ24" s="14"/>
-      <c r="BA24" s="46"/>
+      <c r="BA24" s="43"/>
       <c r="BB24" s="16"/>
       <c r="BC24" s="14"/>
       <c r="BD24" s="14"/>
       <c r="BE24" s="15"/>
-      <c r="BF24" s="45"/>
+      <c r="BF24" s="42"/>
       <c r="BG24" s="14"/>
       <c r="BH24" s="14"/>
-      <c r="BI24" s="46"/>
+      <c r="BI24" s="43"/>
       <c r="BJ24" s="16"/>
       <c r="BK24" s="14"/>
       <c r="BL24" s="14"/>
-      <c r="BM24" s="46"/>
+      <c r="BM24" s="43"/>
     </row>
     <row r="25" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="37"/>
+      <c r="B25" s="34"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
-      <c r="F25" s="37"/>
+      <c r="F25" s="34"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
-      <c r="I25" s="38"/>
+      <c r="I25" s="35"/>
       <c r="J25" s="3"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="2"/>
-      <c r="N25" s="37"/>
+      <c r="N25" s="34"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
-      <c r="Q25" s="38"/>
+      <c r="Q25" s="35"/>
       <c r="R25" s="3"/>
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
-      <c r="U25" s="38"/>
-      <c r="X25" s="37"/>
+      <c r="U25" s="35"/>
+      <c r="X25" s="34"/>
       <c r="Y25" s="1"/>
       <c r="Z25" s="1"/>
       <c r="AA25" s="2"/>
-      <c r="AB25" s="37"/>
+      <c r="AB25" s="34"/>
       <c r="AC25" s="1"/>
       <c r="AD25" s="1"/>
-      <c r="AE25" s="38"/>
+      <c r="AE25" s="35"/>
       <c r="AF25" s="3"/>
       <c r="AG25" s="1"/>
       <c r="AH25" s="1"/>
       <c r="AI25" s="2"/>
-      <c r="AJ25" s="72"/>
-      <c r="AK25" s="73"/>
-      <c r="AL25" s="73"/>
-      <c r="AM25" s="74"/>
-      <c r="AN25" s="76"/>
-      <c r="AO25" s="73"/>
+      <c r="AJ25" s="69"/>
+      <c r="AK25" s="70"/>
+      <c r="AL25" s="70"/>
+      <c r="AM25" s="71"/>
+      <c r="AN25" s="73"/>
+      <c r="AO25" s="70"/>
       <c r="AP25" s="1"/>
-      <c r="AQ25" s="38"/>
-      <c r="AT25" s="37"/>
+      <c r="AQ25" s="35"/>
+      <c r="AT25" s="34"/>
       <c r="AU25" s="1"/>
       <c r="AV25" s="1"/>
       <c r="AW25" s="2"/>
-      <c r="AX25" s="37"/>
+      <c r="AX25" s="34"/>
       <c r="AY25" s="1"/>
       <c r="AZ25" s="1"/>
-      <c r="BA25" s="38"/>
+      <c r="BA25" s="35"/>
       <c r="BB25" s="3"/>
       <c r="BC25" s="1"/>
       <c r="BD25" s="1"/>
       <c r="BE25" s="2"/>
-      <c r="BF25" s="37"/>
+      <c r="BF25" s="34"/>
       <c r="BG25" s="1"/>
       <c r="BH25" s="1"/>
-      <c r="BI25" s="38"/>
+      <c r="BI25" s="35"/>
       <c r="BJ25" s="3"/>
       <c r="BK25" s="1"/>
       <c r="BL25" s="1"/>
-      <c r="BM25" s="38"/>
+      <c r="BM25" s="35"/>
     </row>
     <row r="26" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" s="37"/>
+        <v>37</v>
+      </c>
+      <c r="B26" s="34"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
-      <c r="F26" s="37"/>
+      <c r="F26" s="34"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
-      <c r="I26" s="38"/>
+      <c r="I26" s="35"/>
       <c r="J26" s="3"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="2"/>
-      <c r="N26" s="37"/>
+      <c r="N26" s="34"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
-      <c r="Q26" s="38"/>
+      <c r="Q26" s="35"/>
       <c r="R26" s="3"/>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
-      <c r="U26" s="38"/>
-      <c r="X26" s="37"/>
+      <c r="U26" s="35"/>
+      <c r="X26" s="34"/>
       <c r="Y26" s="1"/>
       <c r="Z26" s="1"/>
       <c r="AA26" s="2"/>
-      <c r="AB26" s="37"/>
+      <c r="AB26" s="34"/>
       <c r="AC26" s="1"/>
       <c r="AD26" s="1"/>
-      <c r="AE26" s="38"/>
+      <c r="AE26" s="35"/>
       <c r="AF26" s="3"/>
       <c r="AG26" s="1"/>
       <c r="AH26" s="1"/>
       <c r="AI26" s="2"/>
-      <c r="AJ26" s="68"/>
-      <c r="AK26" s="69"/>
-      <c r="AL26" s="69"/>
-      <c r="AM26" s="70"/>
-      <c r="AN26" s="71"/>
-      <c r="AO26" s="69"/>
-      <c r="AP26" s="69"/>
-      <c r="AQ26" s="70"/>
-      <c r="AT26" s="37"/>
-      <c r="AU26" s="1"/>
+      <c r="AJ26" s="87"/>
+      <c r="AK26" s="88"/>
+      <c r="AL26" s="88"/>
+      <c r="AM26" s="89"/>
+      <c r="AN26" s="76"/>
+      <c r="AO26" s="74"/>
+      <c r="AP26" s="74"/>
+      <c r="AQ26" s="75"/>
+      <c r="AT26" s="78"/>
+      <c r="AU26" s="74"/>
       <c r="AV26" s="1"/>
       <c r="AW26" s="2"/>
-      <c r="AX26" s="37"/>
+      <c r="AX26" s="34"/>
       <c r="AY26" s="1"/>
       <c r="AZ26" s="1"/>
-      <c r="BA26" s="38"/>
+      <c r="BA26" s="35"/>
       <c r="BB26" s="3"/>
       <c r="BC26" s="1"/>
       <c r="BD26" s="1"/>
       <c r="BE26" s="2"/>
-      <c r="BF26" s="37"/>
+      <c r="BF26" s="34"/>
       <c r="BG26" s="1"/>
       <c r="BH26" s="1"/>
-      <c r="BI26" s="38"/>
+      <c r="BI26" s="35"/>
       <c r="BJ26" s="3"/>
       <c r="BK26" s="1"/>
       <c r="BL26" s="1"/>
-      <c r="BM26" s="38"/>
+      <c r="BM26" s="35"/>
     </row>
     <row r="27" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>17</v>
-      </c>
-      <c r="B27" s="37"/>
+        <v>16</v>
+      </c>
+      <c r="B27" s="34"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="2"/>
-      <c r="F27" s="37"/>
+      <c r="F27" s="34"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
-      <c r="I27" s="38"/>
+      <c r="I27" s="35"/>
       <c r="J27" s="3"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="2"/>
-      <c r="N27" s="37"/>
+      <c r="N27" s="34"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
-      <c r="Q27" s="38"/>
+      <c r="Q27" s="35"/>
       <c r="R27" s="3"/>
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
-      <c r="U27" s="38"/>
-      <c r="X27" s="37"/>
+      <c r="U27" s="35"/>
+      <c r="X27" s="34"/>
       <c r="Y27" s="1"/>
       <c r="Z27" s="1"/>
       <c r="AA27" s="2"/>
-      <c r="AB27" s="37"/>
+      <c r="AB27" s="34"/>
       <c r="AC27" s="1"/>
       <c r="AD27" s="1"/>
-      <c r="AE27" s="38"/>
+      <c r="AE27" s="35"/>
       <c r="AF27" s="3"/>
       <c r="AG27" s="1"/>
       <c r="AH27" s="1"/>
       <c r="AI27" s="2"/>
-      <c r="AJ27" s="37"/>
-      <c r="AK27" s="1"/>
-      <c r="AL27" s="1"/>
-      <c r="AM27" s="38"/>
-      <c r="AN27" s="3"/>
-      <c r="AO27" s="1"/>
-      <c r="AP27" s="73"/>
-      <c r="AQ27" s="74"/>
-      <c r="AT27" s="72"/>
-      <c r="AU27" s="73"/>
-      <c r="AV27" s="73"/>
-      <c r="AW27" s="80"/>
-      <c r="AX27" s="37"/>
+      <c r="AJ27" s="65"/>
+      <c r="AK27" s="66"/>
+      <c r="AL27" s="66"/>
+      <c r="AM27" s="67"/>
+      <c r="AN27" s="68"/>
+      <c r="AO27" s="66"/>
+      <c r="AP27" s="66"/>
+      <c r="AQ27" s="67"/>
+      <c r="AT27" s="34"/>
+      <c r="AU27" s="1"/>
+      <c r="AV27" s="1"/>
+      <c r="AW27" s="2"/>
+      <c r="AX27" s="34"/>
       <c r="AY27" s="1"/>
       <c r="AZ27" s="1"/>
-      <c r="BA27" s="38"/>
+      <c r="BA27" s="35"/>
       <c r="BB27" s="3"/>
       <c r="BC27" s="1"/>
       <c r="BD27" s="1"/>
       <c r="BE27" s="2"/>
-      <c r="BF27" s="37"/>
+      <c r="BF27" s="34"/>
       <c r="BG27" s="1"/>
       <c r="BH27" s="1"/>
-      <c r="BI27" s="38"/>
+      <c r="BI27" s="35"/>
       <c r="BJ27" s="3"/>
       <c r="BK27" s="1"/>
       <c r="BL27" s="1"/>
-      <c r="BM27" s="38"/>
-    </row>
-    <row r="28" spans="1:65" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="25" t="s">
+      <c r="BM27" s="35"/>
+    </row>
+    <row r="28" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="34"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="35"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="34"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="35"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="35"/>
+      <c r="X28" s="34"/>
+      <c r="Y28" s="1"/>
+      <c r="Z28" s="1"/>
+      <c r="AA28" s="2"/>
+      <c r="AB28" s="34"/>
+      <c r="AC28" s="1"/>
+      <c r="AD28" s="1"/>
+      <c r="AE28" s="35"/>
+      <c r="AF28" s="3"/>
+      <c r="AG28" s="1"/>
+      <c r="AH28" s="1"/>
+      <c r="AI28" s="2"/>
+      <c r="AJ28" s="34"/>
+      <c r="AK28" s="1"/>
+      <c r="AL28" s="1"/>
+      <c r="AM28" s="35"/>
+      <c r="AN28" s="3"/>
+      <c r="AO28" s="1"/>
+      <c r="AP28" s="70"/>
+      <c r="AQ28" s="71"/>
+      <c r="AT28" s="69"/>
+      <c r="AU28" s="70"/>
+      <c r="AV28" s="70"/>
+      <c r="AW28" s="77"/>
+      <c r="AX28" s="34"/>
+      <c r="AY28" s="1"/>
+      <c r="AZ28" s="1"/>
+      <c r="BA28" s="35"/>
+      <c r="BB28" s="3"/>
+      <c r="BC28" s="1"/>
+      <c r="BD28" s="1"/>
+      <c r="BE28" s="2"/>
+      <c r="BF28" s="34"/>
+      <c r="BG28" s="1"/>
+      <c r="BH28" s="1"/>
+      <c r="BI28" s="35"/>
+      <c r="BJ28" s="3"/>
+      <c r="BK28" s="1"/>
+      <c r="BL28" s="1"/>
+      <c r="BM28" s="35"/>
+    </row>
+    <row r="29" spans="1:65" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="49"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="50"/>
-      <c r="J28" s="28"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="26"/>
-      <c r="M28" s="27"/>
-      <c r="N28" s="49"/>
-      <c r="O28" s="26"/>
-      <c r="P28" s="26"/>
-      <c r="Q28" s="50"/>
-      <c r="R28" s="28"/>
-      <c r="S28" s="26"/>
-      <c r="T28" s="26"/>
-      <c r="U28" s="50"/>
-      <c r="X28" s="49"/>
-      <c r="Y28" s="26"/>
-      <c r="Z28" s="26"/>
-      <c r="AA28" s="27"/>
-      <c r="AB28" s="49"/>
-      <c r="AC28" s="26"/>
-      <c r="AD28" s="26"/>
-      <c r="AE28" s="50"/>
-      <c r="AF28" s="28"/>
-      <c r="AG28" s="26"/>
-      <c r="AH28" s="26"/>
-      <c r="AI28" s="27"/>
-      <c r="AJ28" s="49"/>
-      <c r="AK28" s="26"/>
-      <c r="AL28" s="26"/>
-      <c r="AM28" s="50"/>
-      <c r="AN28" s="28"/>
-      <c r="AO28" s="26"/>
-      <c r="AP28" s="26"/>
-      <c r="AQ28" s="50"/>
-      <c r="AT28" s="49"/>
-      <c r="AU28" s="26"/>
-      <c r="AV28" s="26"/>
-      <c r="AW28" s="27"/>
-      <c r="AX28" s="49"/>
-      <c r="AY28" s="26"/>
-      <c r="AZ28" s="26"/>
-      <c r="BA28" s="50"/>
-      <c r="BB28" s="28"/>
-      <c r="BC28" s="26"/>
-      <c r="BD28" s="26"/>
-      <c r="BE28" s="27"/>
-      <c r="BF28" s="49"/>
-      <c r="BG28" s="26"/>
-      <c r="BH28" s="26"/>
-      <c r="BI28" s="50"/>
-      <c r="BJ28" s="28"/>
-      <c r="BK28" s="26"/>
-      <c r="BL28" s="26"/>
-      <c r="BM28" s="50"/>
-    </row>
-    <row r="29" spans="1:65" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="21" t="s">
+      <c r="B29" s="46"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="47"/>
+      <c r="J29" s="28"/>
+      <c r="K29" s="26"/>
+      <c r="L29" s="26"/>
+      <c r="M29" s="27"/>
+      <c r="N29" s="46"/>
+      <c r="O29" s="26"/>
+      <c r="P29" s="26"/>
+      <c r="Q29" s="47"/>
+      <c r="R29" s="28"/>
+      <c r="S29" s="26"/>
+      <c r="T29" s="26"/>
+      <c r="U29" s="47"/>
+      <c r="X29" s="46"/>
+      <c r="Y29" s="26"/>
+      <c r="Z29" s="26"/>
+      <c r="AA29" s="27"/>
+      <c r="AB29" s="46"/>
+      <c r="AC29" s="26"/>
+      <c r="AD29" s="26"/>
+      <c r="AE29" s="47"/>
+      <c r="AF29" s="28"/>
+      <c r="AG29" s="26"/>
+      <c r="AH29" s="26"/>
+      <c r="AI29" s="27"/>
+      <c r="AJ29" s="46"/>
+      <c r="AK29" s="26"/>
+      <c r="AL29" s="26"/>
+      <c r="AM29" s="47"/>
+      <c r="AN29" s="28"/>
+      <c r="AO29" s="26"/>
+      <c r="AP29" s="26"/>
+      <c r="AQ29" s="47"/>
+      <c r="AT29" s="46"/>
+      <c r="AU29" s="26"/>
+      <c r="AV29" s="26"/>
+      <c r="AW29" s="27"/>
+      <c r="AX29" s="46"/>
+      <c r="AY29" s="26"/>
+      <c r="AZ29" s="26"/>
+      <c r="BA29" s="47"/>
+      <c r="BB29" s="28"/>
+      <c r="BC29" s="26"/>
+      <c r="BD29" s="26"/>
+      <c r="BE29" s="27"/>
+      <c r="BF29" s="46"/>
+      <c r="BG29" s="26"/>
+      <c r="BH29" s="26"/>
+      <c r="BI29" s="47"/>
+      <c r="BJ29" s="28"/>
+      <c r="BK29" s="26"/>
+      <c r="BL29" s="26"/>
+      <c r="BM29" s="47"/>
+    </row>
+    <row r="30" spans="1:65" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B29" s="43"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="24"/>
-      <c r="K29" s="22"/>
-      <c r="L29" s="22"/>
-      <c r="M29" s="23"/>
-      <c r="N29" s="43"/>
-      <c r="O29" s="22"/>
-      <c r="P29" s="22"/>
-      <c r="Q29" s="44"/>
-      <c r="R29" s="24"/>
-      <c r="S29" s="22"/>
-      <c r="T29" s="22"/>
-      <c r="U29" s="44"/>
-      <c r="X29" s="43"/>
-      <c r="Y29" s="22"/>
-      <c r="Z29" s="22"/>
-      <c r="AA29" s="23"/>
-      <c r="AB29" s="43"/>
-      <c r="AC29" s="22"/>
-      <c r="AD29" s="22"/>
-      <c r="AE29" s="44"/>
-      <c r="AF29" s="24"/>
-      <c r="AG29" s="22"/>
-      <c r="AH29" s="22"/>
-      <c r="AI29" s="23"/>
-      <c r="AJ29" s="43"/>
-      <c r="AK29" s="22"/>
-      <c r="AL29" s="22"/>
-      <c r="AM29" s="44"/>
-      <c r="AN29" s="24"/>
-      <c r="AO29" s="22"/>
-      <c r="AP29" s="22"/>
-      <c r="AQ29" s="44"/>
-      <c r="AT29" s="43"/>
-      <c r="AU29" s="22"/>
-      <c r="AV29" s="22"/>
-      <c r="AW29" s="23"/>
-      <c r="AX29" s="43"/>
-      <c r="AY29" s="22"/>
-      <c r="AZ29" s="22"/>
-      <c r="BA29" s="44"/>
-      <c r="BB29" s="24"/>
-      <c r="BC29" s="22"/>
-      <c r="BD29" s="22"/>
-      <c r="BE29" s="23"/>
-      <c r="BF29" s="43"/>
-      <c r="BG29" s="22"/>
-      <c r="BH29" s="22"/>
-      <c r="BI29" s="44"/>
-      <c r="BJ29" s="24"/>
-      <c r="BK29" s="22"/>
-      <c r="BL29" s="22"/>
-      <c r="BM29" s="44"/>
-    </row>
-    <row r="30" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="B30" s="40"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="41"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="22"/>
+      <c r="L30" s="22"/>
+      <c r="M30" s="23"/>
+      <c r="N30" s="40"/>
+      <c r="O30" s="22"/>
+      <c r="P30" s="22"/>
+      <c r="Q30" s="41"/>
+      <c r="R30" s="24"/>
+      <c r="S30" s="22"/>
+      <c r="T30" s="22"/>
+      <c r="U30" s="41"/>
+      <c r="X30" s="40"/>
+      <c r="Y30" s="22"/>
+      <c r="Z30" s="22"/>
+      <c r="AA30" s="23"/>
+      <c r="AB30" s="40"/>
+      <c r="AC30" s="22"/>
+      <c r="AD30" s="22"/>
+      <c r="AE30" s="41"/>
+      <c r="AF30" s="24"/>
+      <c r="AG30" s="22"/>
+      <c r="AH30" s="22"/>
+      <c r="AI30" s="23"/>
+      <c r="AJ30" s="40"/>
+      <c r="AK30" s="22"/>
+      <c r="AL30" s="22"/>
+      <c r="AM30" s="41"/>
+      <c r="AN30" s="24"/>
+      <c r="AO30" s="22"/>
+      <c r="AP30" s="22"/>
+      <c r="AQ30" s="41"/>
+      <c r="AT30" s="40"/>
+      <c r="AU30" s="22"/>
+      <c r="AV30" s="22"/>
+      <c r="AW30" s="23"/>
+      <c r="AX30" s="40"/>
+      <c r="AY30" s="22"/>
+      <c r="AZ30" s="22"/>
+      <c r="BA30" s="41"/>
+      <c r="BB30" s="24"/>
+      <c r="BC30" s="22"/>
+      <c r="BD30" s="22"/>
+      <c r="BE30" s="23"/>
+      <c r="BF30" s="40"/>
+      <c r="BG30" s="22"/>
+      <c r="BH30" s="22"/>
+      <c r="BI30" s="41"/>
+      <c r="BJ30" s="24"/>
+      <c r="BK30" s="22"/>
+      <c r="BL30" s="22"/>
+      <c r="BM30" s="41"/>
+    </row>
+    <row r="31" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="37"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="37"/>
-      <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="38"/>
-      <c r="R30" s="3"/>
-      <c r="S30" s="1"/>
-      <c r="T30" s="1"/>
-      <c r="U30" s="38"/>
-      <c r="X30" s="37"/>
-      <c r="Y30" s="1"/>
-      <c r="Z30" s="1"/>
-      <c r="AA30" s="2"/>
-      <c r="AB30" s="37"/>
-      <c r="AC30" s="1"/>
-      <c r="AD30" s="1"/>
-      <c r="AE30" s="38"/>
-      <c r="AF30" s="3"/>
-      <c r="AG30" s="1"/>
-      <c r="AH30" s="1"/>
-      <c r="AI30" s="2"/>
-      <c r="AJ30" s="37"/>
-      <c r="AK30" s="1"/>
-      <c r="AL30" s="1"/>
-      <c r="AM30" s="38"/>
-      <c r="AN30" s="3"/>
-      <c r="AO30" s="1"/>
-      <c r="AP30" s="1"/>
-      <c r="AQ30" s="38"/>
-      <c r="AT30" s="68"/>
-      <c r="AU30" s="69"/>
-      <c r="AV30" s="69"/>
-      <c r="AW30" s="75"/>
-      <c r="AX30" s="37"/>
-      <c r="AY30" s="1"/>
-      <c r="AZ30" s="1"/>
-      <c r="BA30" s="38"/>
-      <c r="BB30" s="3"/>
-      <c r="BC30" s="1"/>
-      <c r="BD30" s="1"/>
-      <c r="BE30" s="2"/>
-      <c r="BF30" s="37"/>
-      <c r="BG30" s="1"/>
-      <c r="BH30" s="1"/>
-      <c r="BI30" s="38"/>
-      <c r="BJ30" s="3"/>
-      <c r="BK30" s="1"/>
-      <c r="BL30" s="1"/>
-      <c r="BM30" s="38"/>
-    </row>
-    <row r="31" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="B31" s="34"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="35"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="34"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="35"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="35"/>
+      <c r="X31" s="34"/>
+      <c r="Y31" s="1"/>
+      <c r="Z31" s="1"/>
+      <c r="AA31" s="2"/>
+      <c r="AB31" s="34"/>
+      <c r="AC31" s="1"/>
+      <c r="AD31" s="1"/>
+      <c r="AE31" s="35"/>
+      <c r="AF31" s="3"/>
+      <c r="AG31" s="1"/>
+      <c r="AH31" s="1"/>
+      <c r="AI31" s="2"/>
+      <c r="AJ31" s="34"/>
+      <c r="AK31" s="1"/>
+      <c r="AL31" s="1"/>
+      <c r="AM31" s="35"/>
+      <c r="AN31" s="3"/>
+      <c r="AO31" s="1"/>
+      <c r="AP31" s="1"/>
+      <c r="AQ31" s="35"/>
+      <c r="AT31" s="65"/>
+      <c r="AU31" s="66"/>
+      <c r="AV31" s="66"/>
+      <c r="AW31" s="72"/>
+      <c r="AX31" s="34"/>
+      <c r="AY31" s="1"/>
+      <c r="AZ31" s="1"/>
+      <c r="BA31" s="35"/>
+      <c r="BB31" s="3"/>
+      <c r="BC31" s="1"/>
+      <c r="BD31" s="1"/>
+      <c r="BE31" s="2"/>
+      <c r="BF31" s="34"/>
+      <c r="BG31" s="1"/>
+      <c r="BH31" s="1"/>
+      <c r="BI31" s="35"/>
+      <c r="BJ31" s="3"/>
+      <c r="BK31" s="1"/>
+      <c r="BL31" s="1"/>
+      <c r="BM31" s="35"/>
+    </row>
+    <row r="32" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="51"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="52"/>
-      <c r="E31" s="55"/>
-      <c r="F31" s="51"/>
-      <c r="G31" s="52"/>
-      <c r="H31" s="52"/>
-      <c r="I31" s="53"/>
-      <c r="J31" s="57"/>
-      <c r="K31" s="52"/>
-      <c r="L31" s="52"/>
-      <c r="M31" s="55"/>
-      <c r="N31" s="51"/>
-      <c r="O31" s="52"/>
-      <c r="P31" s="52"/>
-      <c r="Q31" s="53"/>
-      <c r="R31" s="57"/>
-      <c r="S31" s="52"/>
-      <c r="T31" s="52"/>
-      <c r="U31" s="53"/>
-      <c r="X31" s="51"/>
-      <c r="Y31" s="52"/>
-      <c r="Z31" s="52"/>
-      <c r="AA31" s="55"/>
-      <c r="AB31" s="51"/>
-      <c r="AC31" s="52"/>
-      <c r="AD31" s="52"/>
-      <c r="AE31" s="53"/>
-      <c r="AF31" s="57"/>
-      <c r="AG31" s="52"/>
-      <c r="AH31" s="52"/>
-      <c r="AI31" s="55"/>
-      <c r="AJ31" s="51"/>
-      <c r="AK31" s="52"/>
-      <c r="AL31" s="52"/>
-      <c r="AM31" s="53"/>
-      <c r="AN31" s="57"/>
-      <c r="AO31" s="52"/>
-      <c r="AP31" s="52"/>
-      <c r="AQ31" s="53"/>
-      <c r="AT31" s="83"/>
-      <c r="AU31" s="84"/>
-      <c r="AV31" s="84"/>
-      <c r="AW31" s="85"/>
-      <c r="AX31" s="83"/>
-      <c r="AY31" s="84"/>
-      <c r="AZ31" s="84"/>
-      <c r="BA31" s="86"/>
-      <c r="BB31" s="57"/>
-      <c r="BC31" s="52"/>
-      <c r="BD31" s="52"/>
-      <c r="BE31" s="55"/>
-      <c r="BF31" s="51"/>
-      <c r="BG31" s="52"/>
-      <c r="BH31" s="52"/>
-      <c r="BI31" s="53"/>
-      <c r="BJ31" s="57"/>
-      <c r="BK31" s="52"/>
-      <c r="BL31" s="52"/>
-      <c r="BM31" s="53"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="B32" s="48"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="52"/>
+      <c r="F32" s="48"/>
+      <c r="G32" s="49"/>
+      <c r="H32" s="49"/>
+      <c r="I32" s="50"/>
+      <c r="J32" s="54"/>
+      <c r="K32" s="49"/>
+      <c r="L32" s="49"/>
+      <c r="M32" s="52"/>
+      <c r="N32" s="48"/>
+      <c r="O32" s="49"/>
+      <c r="P32" s="49"/>
+      <c r="Q32" s="50"/>
+      <c r="R32" s="54"/>
+      <c r="S32" s="49"/>
+      <c r="T32" s="49"/>
+      <c r="U32" s="50"/>
+      <c r="X32" s="48"/>
+      <c r="Y32" s="49"/>
+      <c r="Z32" s="49"/>
+      <c r="AA32" s="52"/>
+      <c r="AB32" s="48"/>
+      <c r="AC32" s="49"/>
+      <c r="AD32" s="49"/>
+      <c r="AE32" s="50"/>
+      <c r="AF32" s="54"/>
+      <c r="AG32" s="49"/>
+      <c r="AH32" s="49"/>
+      <c r="AI32" s="52"/>
+      <c r="AJ32" s="48"/>
+      <c r="AK32" s="49"/>
+      <c r="AL32" s="49"/>
+      <c r="AM32" s="50"/>
+      <c r="AN32" s="54"/>
+      <c r="AO32" s="49"/>
+      <c r="AP32" s="49"/>
+      <c r="AQ32" s="50"/>
+      <c r="AT32" s="90"/>
+      <c r="AU32" s="91"/>
+      <c r="AV32" s="81"/>
+      <c r="AW32" s="82"/>
+      <c r="AX32" s="80"/>
+      <c r="AY32" s="81"/>
+      <c r="AZ32" s="81"/>
+      <c r="BA32" s="83"/>
+      <c r="BB32" s="54"/>
+      <c r="BC32" s="49"/>
+      <c r="BD32" s="49"/>
+      <c r="BE32" s="52"/>
+      <c r="BF32" s="48"/>
+      <c r="BG32" s="49"/>
+      <c r="BH32" s="49"/>
+      <c r="BI32" s="50"/>
+      <c r="BJ32" s="54"/>
+      <c r="BK32" s="49"/>
+      <c r="BL32" s="49"/>
+      <c r="BM32" s="50"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="61" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="58" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="62" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="59" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="56" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="60" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="57" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Mise en page du planning pour exportation au format PDF
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Joel_Vaucher\INF2-b\HesETE-p2-Vaucher\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitsWin\HesETE-p2-Vaucher\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$BM$43</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -143,10 +146,18 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -523,7 +534,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -608,6 +619,11 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -617,11 +633,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -715,6 +727,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -750,6 +779,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -902,11 +948,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:BM43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AO35" sqref="AO35"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,97 +963,98 @@
     <col min="1" max="1" width="34.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="84">
+    <row r="1" spans="1:65" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="92"/>
+      <c r="B1" s="89">
         <v>42604</v>
       </c>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="84">
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="89">
         <v>42605</v>
       </c>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="84">
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="89">
         <v>42606</v>
       </c>
-      <c r="K1" s="85"/>
-      <c r="L1" s="85"/>
-      <c r="M1" s="86"/>
-      <c r="N1" s="84">
+      <c r="K1" s="90"/>
+      <c r="L1" s="90"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="89">
         <v>42607</v>
       </c>
-      <c r="O1" s="85"/>
-      <c r="P1" s="85"/>
-      <c r="Q1" s="86"/>
-      <c r="R1" s="84">
+      <c r="O1" s="90"/>
+      <c r="P1" s="90"/>
+      <c r="Q1" s="91"/>
+      <c r="R1" s="89">
         <v>42608</v>
       </c>
-      <c r="S1" s="85"/>
-      <c r="T1" s="85"/>
-      <c r="U1" s="86"/>
-      <c r="X1" s="84">
+      <c r="S1" s="90"/>
+      <c r="T1" s="90"/>
+      <c r="U1" s="91"/>
+      <c r="X1" s="89">
         <v>42611</v>
       </c>
-      <c r="Y1" s="85"/>
-      <c r="Z1" s="85"/>
-      <c r="AA1" s="86"/>
-      <c r="AB1" s="84">
+      <c r="Y1" s="90"/>
+      <c r="Z1" s="90"/>
+      <c r="AA1" s="91"/>
+      <c r="AB1" s="89">
         <v>42612</v>
       </c>
-      <c r="AC1" s="85"/>
-      <c r="AD1" s="85"/>
-      <c r="AE1" s="86"/>
-      <c r="AF1" s="84">
+      <c r="AC1" s="90"/>
+      <c r="AD1" s="90"/>
+      <c r="AE1" s="91"/>
+      <c r="AF1" s="89">
         <v>42613</v>
       </c>
-      <c r="AG1" s="85"/>
-      <c r="AH1" s="85"/>
-      <c r="AI1" s="86"/>
-      <c r="AJ1" s="84">
+      <c r="AG1" s="90"/>
+      <c r="AH1" s="90"/>
+      <c r="AI1" s="91"/>
+      <c r="AJ1" s="89">
         <v>42614</v>
       </c>
-      <c r="AK1" s="85"/>
-      <c r="AL1" s="85"/>
-      <c r="AM1" s="86"/>
-      <c r="AN1" s="84">
+      <c r="AK1" s="90"/>
+      <c r="AL1" s="90"/>
+      <c r="AM1" s="91"/>
+      <c r="AN1" s="89">
         <v>42615</v>
       </c>
-      <c r="AO1" s="85"/>
-      <c r="AP1" s="85"/>
-      <c r="AQ1" s="86"/>
-      <c r="AT1" s="84">
+      <c r="AO1" s="90"/>
+      <c r="AP1" s="90"/>
+      <c r="AQ1" s="91"/>
+      <c r="AT1" s="89">
         <v>42618</v>
       </c>
-      <c r="AU1" s="85"/>
-      <c r="AV1" s="85"/>
-      <c r="AW1" s="86"/>
-      <c r="AX1" s="84">
+      <c r="AU1" s="90"/>
+      <c r="AV1" s="90"/>
+      <c r="AW1" s="91"/>
+      <c r="AX1" s="89">
         <v>42619</v>
       </c>
-      <c r="AY1" s="85"/>
-      <c r="AZ1" s="85"/>
-      <c r="BA1" s="86"/>
-      <c r="BB1" s="84">
+      <c r="AY1" s="90"/>
+      <c r="AZ1" s="90"/>
+      <c r="BA1" s="91"/>
+      <c r="BB1" s="89">
         <v>42620</v>
       </c>
-      <c r="BC1" s="85"/>
-      <c r="BD1" s="85"/>
-      <c r="BE1" s="86"/>
-      <c r="BF1" s="84">
+      <c r="BC1" s="90"/>
+      <c r="BD1" s="90"/>
+      <c r="BE1" s="91"/>
+      <c r="BF1" s="89">
         <v>42621</v>
       </c>
-      <c r="BG1" s="85"/>
-      <c r="BH1" s="85"/>
-      <c r="BI1" s="86"/>
-      <c r="BJ1" s="84">
+      <c r="BG1" s="90"/>
+      <c r="BH1" s="90"/>
+      <c r="BI1" s="91"/>
+      <c r="BJ1" s="89">
         <v>42622</v>
       </c>
-      <c r="BK1" s="85"/>
-      <c r="BL1" s="85"/>
-      <c r="BM1" s="86"/>
+      <c r="BK1" s="90"/>
+      <c r="BL1" s="90"/>
+      <c r="BM1" s="91"/>
     </row>
     <row r="2" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="29" t="s">
@@ -2659,10 +2709,10 @@
       <c r="AG26" s="1"/>
       <c r="AH26" s="1"/>
       <c r="AI26" s="2"/>
-      <c r="AJ26" s="87"/>
-      <c r="AK26" s="88"/>
-      <c r="AL26" s="88"/>
-      <c r="AM26" s="89"/>
+      <c r="AJ26" s="84"/>
+      <c r="AK26" s="85"/>
+      <c r="AL26" s="85"/>
+      <c r="AM26" s="86"/>
       <c r="AN26" s="76"/>
       <c r="AO26" s="74"/>
       <c r="AP26" s="74"/>
@@ -3057,8 +3107,8 @@
       <c r="AO32" s="49"/>
       <c r="AP32" s="49"/>
       <c r="AQ32" s="50"/>
-      <c r="AT32" s="90"/>
-      <c r="AU32" s="91"/>
+      <c r="AT32" s="87"/>
+      <c r="AU32" s="88"/>
       <c r="AV32" s="81"/>
       <c r="AW32" s="82"/>
       <c r="AX32" s="80"/>
@@ -3141,7 +3191,15 @@
     <mergeCell ref="AJ1:AM1"/>
     <mergeCell ref="AN1:AQ1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="51" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;LPlanning
+Travel Time Guy&amp;RVaucher Joel
+Ombang Ndo Charles
+Rodrigues Lourenço Daniel</oddHeader>
+    <oddFooter>&amp;L&amp;D&amp;R&amp;P/&amp;N</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>